<commit_message>
Tried to simulate testing credibility rate, but it is not working so far. Attempting to use monte carlo simulation for confidence interval approach for mdm.
</commit_message>
<xml_diff>
--- a/mdm_t/atherosclerosis_review.xlsx
+++ b/mdm_t/atherosclerosis_review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\CodeProjects\ACE\mdm_z\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\CodeProjects\ACE\mdm_t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A887F96F-A7A1-43D3-9E05-48A04DBC1F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD22590-D4C5-41C4-A971-CF95B24B58A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27975" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="2" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chol Null" sheetId="2" r:id="rId1"/>
@@ -10149,8 +10149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7F0DCD-E304-4017-B7AF-97A0978AC45D}">
   <dimension ref="A1:AK48"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10267,10 +10267,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="16">
-        <v>0.121593125828345</v>
+        <v>0.13043809731668399</v>
       </c>
       <c r="C3" s="30">
-        <v>0.43489703122732398</v>
+        <v>0.46617672599795501</v>
       </c>
       <c r="D3" s="34">
         <v>-0.81536804330346402</v>
@@ -10336,10 +10336,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="50">
-        <v>0.17184334993397399</v>
+        <v>0.182987513469201</v>
       </c>
       <c r="C4" s="104">
-        <v>224.70797058015799</v>
+        <v>242.534664608041</v>
       </c>
       <c r="D4" s="118">
         <v>-0.47254624603545098</v>
@@ -10402,10 +10402,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="16">
-        <v>0.219693893758835</v>
+        <v>0.26420001124753001</v>
       </c>
       <c r="C5" s="30">
-        <v>0.53182707887899106</v>
+        <v>0.58346606311361404</v>
       </c>
       <c r="D5" s="34">
         <v>2.28994290098559E-2</v>
@@ -10468,10 +10468,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="50">
-        <v>0.25081372019273901</v>
+        <v>0.29182974321097899</v>
       </c>
       <c r="C6" s="120">
-        <v>35.198852708612897</v>
+        <v>36.302317354308599</v>
       </c>
       <c r="D6" s="118">
         <v>0.339813833015292</v>
@@ -10532,10 +10532,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="16">
-        <v>0.30345351551815197</v>
+        <v>0.31276024065841501</v>
       </c>
       <c r="C7" s="30">
-        <v>35.153294791160398</v>
+        <v>36.360994422495601</v>
       </c>
       <c r="D7" s="34">
         <v>-0.40808436225286598</v>
@@ -10600,10 +10600,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="50">
-        <v>0.30860369698662699</v>
+        <v>0.33734987809688799</v>
       </c>
       <c r="C8" s="104">
-        <v>788.42874293045998</v>
+        <v>833.60407214252302</v>
       </c>
       <c r="D8" s="118">
         <v>0.89209842929858996</v>
@@ -10666,10 +10666,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="16">
-        <v>0.44229019357833699</v>
+        <v>0.51915686072365597</v>
       </c>
       <c r="C9" s="28">
-        <v>575.65772240748095</v>
+        <v>635.99117263386904</v>
       </c>
       <c r="D9" s="34">
         <v>-9.7892748415847802E-2</v>
@@ -10733,10 +10733,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="50">
-        <v>0.79871378003520699</v>
+        <v>0.91116231634290201</v>
       </c>
       <c r="C10" s="104">
-        <v>486.60516347500698</v>
+        <v>510.73127368201398</v>
       </c>
       <c r="D10" s="118">
         <v>0.91661505293428103</v>
@@ -10799,10 +10799,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="16">
-        <v>1.5427763928473599</v>
+        <v>2.02225888187224</v>
       </c>
       <c r="C11" s="30">
-        <v>11.002317590911201</v>
+        <v>11.5179506416553</v>
       </c>
       <c r="D11" s="34">
         <v>0.52932779470774505</v>
@@ -13498,8 +13498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B673FAB6-1E3C-4258-9C8D-D9DBE685A34B}">
   <dimension ref="A1:AK44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C11"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9" x14ac:dyDescent="0.15"/>
@@ -13631,10 +13631,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="16">
-        <v>0.15587183086280601</v>
+        <v>0.15179126609969301</v>
       </c>
       <c r="C3" s="34">
-        <v>6.8478424111484504</v>
+        <v>7.1268826017500304</v>
       </c>
       <c r="D3" s="96">
         <v>0.61999379158845302</v>
@@ -13699,10 +13699,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="50">
-        <v>0.20303818219409001</v>
+        <v>0.24129939710994899</v>
       </c>
       <c r="C4" s="44">
-        <v>146293.86068285399</v>
+        <v>158840.570149281</v>
       </c>
       <c r="D4" s="97">
         <v>3.5713564070074102E-2</v>
@@ -13765,10 +13765,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="51">
-        <v>0.26359851262496098</v>
+        <v>0.31491948549316001</v>
       </c>
       <c r="C5" s="94">
-        <v>109228.62148842</v>
+        <v>115266.14071585301</v>
       </c>
       <c r="D5" s="98">
         <v>5.0486469068246699E-2</v>
@@ -13832,10 +13832,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="16">
-        <v>0.32910520157054102</v>
+        <v>0.31061758132699901</v>
       </c>
       <c r="C6" s="28">
-        <v>126.021317239962</v>
+        <v>127.23067180345799</v>
       </c>
       <c r="D6" s="96">
         <v>0.91323124927187205</v>
@@ -13899,10 +13899,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="51">
-        <v>0.50762085262478696</v>
+        <v>0.633079824678911</v>
       </c>
       <c r="C7" s="95">
-        <v>15.0016629188304</v>
+        <v>16.177375293757699</v>
       </c>
       <c r="D7" s="98">
         <v>0.39130715079531098</v>
@@ -13966,10 +13966,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="16">
-        <v>1.0902953689300201</v>
+        <v>1.09857171516531</v>
       </c>
       <c r="C8" s="34">
-        <v>0.655449359381305</v>
+        <v>0.71020712681328102</v>
       </c>
       <c r="D8" s="96">
         <v>0.25180073430266697</v>
@@ -14033,10 +14033,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="51">
-        <v>1.32890473186248</v>
+        <v>1.06146056606671</v>
       </c>
       <c r="C9" s="94">
-        <v>33.3235397238236</v>
+        <v>34.608572305934999</v>
       </c>
       <c r="D9" s="98">
         <v>0.12847995194645101</v>
@@ -14101,10 +14101,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="50">
-        <v>2.2018381936729998</v>
+        <v>3.99759047989915</v>
       </c>
       <c r="C10" s="94">
-        <v>473501.849983714</v>
+        <v>749292.30353048595</v>
       </c>
       <c r="D10" s="97">
         <v>3.9523876652813497E-2</v>
@@ -14168,10 +14168,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="51">
-        <v>5.02369447699063</v>
+        <v>4.8342169763688796</v>
       </c>
       <c r="C11" s="94">
-        <v>17513.883164908399</v>
+        <v>17727.333292926902</v>
       </c>
       <c r="D11" s="98">
         <v>0.57883864704215804</v>

</xml_diff>

<commit_message>
Recomputed r_delta_m applied examples and continued with credibility testing.
</commit_message>
<xml_diff>
--- a/mdm_t/atherosclerosis_review.xlsx
+++ b/mdm_t/atherosclerosis_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\CodeProjects\ACE\mdm_t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD22590-D4C5-41C4-A971-CF95B24B58A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E7C863-5128-4FDB-9351-65C6EBC57DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
+    <workbookView xWindow="33015" yWindow="2460" windowWidth="20910" windowHeight="11835" activeTab="2" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chol Null" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="439">
   <si>
     <t>Measure</t>
   </si>
@@ -4815,6 +4815,82 @@
   </si>
   <si>
     <t>AE</t>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>̅</t>
+    </r>
+  </si>
+  <si>
+    <t>Group X</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>̅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Group Y</t>
   </si>
 </sst>
 </file>
@@ -5149,7 +5225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5284,12 +5360,6 @@
     <xf numFmtId="165" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5326,9 +5396,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="12" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5469,6 +5536,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10149,8 +10219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7F0DCD-E304-4017-B7AF-97A0978AC45D}">
   <dimension ref="A1:AK48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10201,64 +10271,64 @@
     </row>
     <row r="2" spans="1:37" s="47" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53"/>
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="111" t="s">
         <v>363</v>
       </c>
-      <c r="C2" s="114" t="s">
+      <c r="C2" s="111" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="114" t="s">
+      <c r="D2" s="111" t="s">
         <v>368</v>
       </c>
-      <c r="E2" s="114" t="s">
+      <c r="E2" s="111" t="s">
         <v>406</v>
       </c>
-      <c r="F2" s="114" t="s">
+      <c r="F2" s="111" t="s">
         <v>405</v>
       </c>
-      <c r="G2" s="114" t="s">
+      <c r="G2" s="111" t="s">
         <v>367</v>
       </c>
-      <c r="H2" s="114" t="s">
+      <c r="H2" s="111" t="s">
         <v>361</v>
       </c>
-      <c r="I2" s="115" t="s">
-        <v>422</v>
-      </c>
-      <c r="J2" s="116" t="s">
-        <v>427</v>
-      </c>
-      <c r="K2" s="116" t="s">
-        <v>428</v>
-      </c>
-      <c r="L2" s="116" t="s">
-        <v>423</v>
-      </c>
-      <c r="M2" s="115" t="s">
-        <v>429</v>
-      </c>
-      <c r="N2" s="116" t="s">
-        <v>424</v>
-      </c>
-      <c r="O2" s="116" t="s">
-        <v>425</v>
-      </c>
-      <c r="P2" s="116" t="s">
-        <v>426</v>
-      </c>
-      <c r="Q2" s="116" t="s">
+      <c r="I2" s="112" t="s">
+        <v>432</v>
+      </c>
+      <c r="J2" s="113" t="s">
+        <v>431</v>
+      </c>
+      <c r="K2" s="113" t="s">
+        <v>436</v>
+      </c>
+      <c r="L2" s="113" t="s">
+        <v>433</v>
+      </c>
+      <c r="M2" s="112" t="s">
+        <v>438</v>
+      </c>
+      <c r="N2" s="113" t="s">
+        <v>434</v>
+      </c>
+      <c r="O2" s="113" t="s">
+        <v>435</v>
+      </c>
+      <c r="P2" s="113" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q2" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="116" t="s">
+      <c r="R2" s="113" t="s">
         <v>362</v>
       </c>
-      <c r="S2" s="114" t="s">
+      <c r="S2" s="111" t="s">
         <v>303</v>
       </c>
-      <c r="T2" s="117" t="s">
+      <c r="T2" s="114" t="s">
         <v>172</v>
       </c>
-      <c r="U2" s="114" t="s">
+      <c r="U2" s="111" t="s">
         <v>430</v>
       </c>
     </row>
@@ -10267,10 +10337,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="16">
-        <v>0.13043809731668399</v>
+        <v>0.13019237383551699</v>
       </c>
       <c r="C3" s="30">
-        <v>0.46617672599795501</v>
+        <v>0.47260005697817697</v>
       </c>
       <c r="D3" s="34">
         <v>-0.81536804330346402</v>
@@ -10284,7 +10354,7 @@
       <c r="G3" s="34">
         <v>0.851980223093454</v>
       </c>
-      <c r="H3" s="88">
+      <c r="H3" s="85">
         <f t="shared" ref="H3:H11" si="0">-(J3-N3)/J3</f>
         <v>-5.5072463768116052E-2</v>
       </c>
@@ -10326,7 +10396,7 @@
       <c r="T3" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="U3" s="99" t="s">
+      <c r="U3" s="96" t="s">
         <v>420</v>
       </c>
       <c r="Z3" s="48"/>
@@ -10336,24 +10406,24 @@
         <v>2</v>
       </c>
       <c r="B4" s="50">
-        <v>0.182987513469201</v>
-      </c>
-      <c r="C4" s="104">
-        <v>242.534664608041</v>
-      </c>
-      <c r="D4" s="118">
+        <v>0.19260782918090599</v>
+      </c>
+      <c r="C4" s="101">
+        <v>247.30405964305601</v>
+      </c>
+      <c r="D4" s="115">
         <v>-0.47254624603545098</v>
       </c>
-      <c r="E4" s="118">
+      <c r="E4" s="115">
         <v>0.40148668462064402</v>
       </c>
-      <c r="F4" s="118">
+      <c r="F4" s="115">
         <v>0.79351932236539702</v>
       </c>
-      <c r="G4" s="118">
+      <c r="G4" s="115">
         <v>0.56906030560818099</v>
       </c>
-      <c r="H4" s="119">
+      <c r="H4" s="116">
         <f t="shared" si="0"/>
         <v>-5.7553956834532377E-2</v>
       </c>
@@ -10363,7 +10433,7 @@
       <c r="J4" s="44">
         <v>1251</v>
       </c>
-      <c r="K4" s="104">
+      <c r="K4" s="101">
         <v>161.1</v>
       </c>
       <c r="L4" s="44">
@@ -10375,7 +10445,7 @@
       <c r="N4" s="44">
         <v>1179</v>
       </c>
-      <c r="O4" s="104">
+      <c r="O4" s="101">
         <v>143.1</v>
       </c>
       <c r="P4" s="44">
@@ -10393,7 +10463,7 @@
       <c r="T4" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="U4" s="107" t="s">
+      <c r="U4" s="104" t="s">
         <v>420</v>
       </c>
     </row>
@@ -10402,10 +10472,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="16">
-        <v>0.26420001124753001</v>
+        <v>0.26823249855064502</v>
       </c>
       <c r="C5" s="30">
-        <v>0.58346606311361404</v>
+        <v>0.60108092699055404</v>
       </c>
       <c r="D5" s="34">
         <v>2.28994290098559E-2</v>
@@ -10419,7 +10489,7 @@
       <c r="G5" s="34">
         <v>0.45717000666624003</v>
       </c>
-      <c r="H5" s="88">
+      <c r="H5" s="85">
         <f t="shared" si="0"/>
         <v>4.3668122270741428E-3</v>
       </c>
@@ -10468,46 +10538,46 @@
         <v>4</v>
       </c>
       <c r="B6" s="50">
-        <v>0.29182974321097899</v>
-      </c>
-      <c r="C6" s="120">
-        <v>36.302317354308599</v>
-      </c>
-      <c r="D6" s="118">
+        <v>0.29776060038375401</v>
+      </c>
+      <c r="C6" s="117">
+        <v>37.184206948451099</v>
+      </c>
+      <c r="D6" s="115">
         <v>0.339813833015292</v>
       </c>
-      <c r="E6" s="118">
+      <c r="E6" s="115">
         <v>0.481528550865643</v>
       </c>
-      <c r="F6" s="118">
+      <c r="F6" s="115">
         <v>0.78112699963690202</v>
       </c>
-      <c r="G6" s="118">
+      <c r="G6" s="115">
         <v>0.49667580631239</v>
       </c>
-      <c r="H6" s="119">
+      <c r="H6" s="116">
         <f t="shared" si="0"/>
         <v>7.0921985815602842E-2</v>
       </c>
-      <c r="I6" s="121" t="s">
+      <c r="I6" s="118" t="s">
         <v>240</v>
       </c>
       <c r="J6" s="44">
         <v>141</v>
       </c>
-      <c r="K6" s="104">
+      <c r="K6" s="101">
         <v>34</v>
       </c>
       <c r="L6" s="44">
         <v>8</v>
       </c>
-      <c r="M6" s="121" t="s">
+      <c r="M6" s="118" t="s">
         <v>241</v>
       </c>
       <c r="N6" s="44">
         <v>151</v>
       </c>
-      <c r="O6" s="104">
+      <c r="O6" s="101">
         <v>24</v>
       </c>
       <c r="P6" s="44">
@@ -10532,10 +10602,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="16">
-        <v>0.31276024065841501</v>
+        <v>0.31606907468118001</v>
       </c>
       <c r="C7" s="30">
-        <v>36.360994422495601</v>
+        <v>35.989193510506901</v>
       </c>
       <c r="D7" s="34">
         <v>-0.40808436225286598</v>
@@ -10549,7 +10619,7 @@
       <c r="G7" s="34">
         <v>0.55115140592292</v>
       </c>
-      <c r="H7" s="88">
+      <c r="H7" s="85">
         <f t="shared" ref="H7" si="1">-(J7-N7)/J7</f>
         <v>-0.11132254995242616</v>
       </c>
@@ -10591,7 +10661,7 @@
       <c r="T7" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="U7" s="99" t="s">
+      <c r="U7" s="96" t="s">
         <v>420</v>
       </c>
     </row>
@@ -10600,24 +10670,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="50">
-        <v>0.33734987809688799</v>
-      </c>
-      <c r="C8" s="104">
-        <v>833.60407214252302</v>
-      </c>
-      <c r="D8" s="118">
+        <v>0.33388866200202799</v>
+      </c>
+      <c r="C8" s="101">
+        <v>819.70352162230699</v>
+      </c>
+      <c r="D8" s="115">
         <v>0.89209842929858996</v>
       </c>
-      <c r="E8" s="118">
+      <c r="E8" s="115">
         <v>0.157069703569087</v>
       </c>
-      <c r="F8" s="118">
+      <c r="F8" s="115">
         <v>0.94722941186061105</v>
       </c>
-      <c r="G8" s="118">
+      <c r="G8" s="115">
         <v>1.12553466960461</v>
       </c>
-      <c r="H8" s="119">
+      <c r="H8" s="116">
         <f>-(J8-N8)/J8</f>
         <v>0.14217633042096903</v>
       </c>
@@ -10657,7 +10727,7 @@
       <c r="T8" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="U8" s="107" t="s">
+      <c r="U8" s="104" t="s">
         <v>420</v>
       </c>
     </row>
@@ -10666,10 +10736,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="16">
-        <v>0.51915686072365597</v>
+        <v>0.49913975212442901</v>
       </c>
       <c r="C9" s="28">
-        <v>635.99117263386904</v>
+        <v>639.08595078976498</v>
       </c>
       <c r="D9" s="34">
         <v>-9.7892748415847802E-2</v>
@@ -10683,7 +10753,7 @@
       <c r="G9" s="34">
         <v>0.43322506677697697</v>
       </c>
-      <c r="H9" s="88">
+      <c r="H9" s="85">
         <v>-2.3970037453183522E-2</v>
       </c>
       <c r="I9" s="14" t="s">
@@ -10724,7 +10794,7 @@
       <c r="T9" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="U9" s="99" t="s">
+      <c r="U9" s="96" t="s">
         <v>420</v>
       </c>
     </row>
@@ -10733,24 +10803,24 @@
         <v>8</v>
       </c>
       <c r="B10" s="50">
-        <v>0.91116231634290201</v>
-      </c>
-      <c r="C10" s="104">
-        <v>510.73127368201398</v>
-      </c>
-      <c r="D10" s="118">
+        <v>0.90309472501463095</v>
+      </c>
+      <c r="C10" s="101">
+        <v>508.062721055868</v>
+      </c>
+      <c r="D10" s="115">
         <v>0.91661505293428103</v>
       </c>
-      <c r="E10" s="118">
+      <c r="E10" s="115">
         <v>0.269707626815824</v>
       </c>
-      <c r="F10" s="118">
+      <c r="F10" s="115">
         <v>0.92710580411542498</v>
       </c>
-      <c r="G10" s="118">
+      <c r="G10" s="115">
         <v>1.00171580801154</v>
       </c>
-      <c r="H10" s="119">
+      <c r="H10" s="116">
         <f t="shared" si="0"/>
         <v>0.30633802816901406</v>
       </c>
@@ -10760,7 +10830,7 @@
       <c r="J10" s="44">
         <v>568</v>
       </c>
-      <c r="K10" s="104">
+      <c r="K10" s="101">
         <f>(601-J10)*SQRT(L10)</f>
         <v>80.833161511844864</v>
       </c>
@@ -10799,10 +10869,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="16">
-        <v>2.02225888187224</v>
+        <v>2.02690768158753</v>
       </c>
       <c r="C11" s="30">
-        <v>11.5179506416553</v>
+        <v>11.699378345422099</v>
       </c>
       <c r="D11" s="34">
         <v>0.52932779470774505</v>
@@ -10816,7 +10886,7 @@
       <c r="G11" s="34">
         <v>0.62062434824087698</v>
       </c>
-      <c r="H11" s="88">
+      <c r="H11" s="85">
         <f t="shared" si="0"/>
         <v>0.36607142857142871</v>
       </c>
@@ -10856,20 +10926,20 @@
       <c r="T11" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="U11" s="99" t="s">
+      <c r="U11" s="96" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" s="53"/>
-      <c r="B12" s="100"/>
+      <c r="B12" s="97"/>
       <c r="C12" s="34"/>
       <c r="H12" s="16"/>
       <c r="I12" s="33"/>
       <c r="K12" s="28"/>
       <c r="M12" s="17"/>
       <c r="O12" s="30"/>
-      <c r="U12" s="99"/>
+      <c r="U12" s="96"/>
       <c r="V12" s="23"/>
       <c r="W12" s="23"/>
       <c r="X12" s="23"/>
@@ -10894,14 +10964,14 @@
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
-      <c r="H13" s="88"/>
+      <c r="H13" s="85"/>
       <c r="I13" s="33"/>
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
       <c r="M13" s="17"/>
       <c r="O13" s="28"/>
       <c r="Q13" s="29"/>
-      <c r="U13" s="99"/>
+      <c r="U13" s="96"/>
       <c r="V13" s="23"/>
       <c r="W13" s="23"/>
       <c r="X13" s="23"/>
@@ -11012,11 +11082,11 @@
       <c r="W16" s="22"/>
       <c r="X16" s="22"/>
       <c r="Y16" s="22"/>
-      <c r="Z16" s="85"/>
-      <c r="AA16" s="85"/>
-      <c r="AB16" s="85"/>
-      <c r="AC16" s="85"/>
-      <c r="AD16" s="85"/>
+      <c r="Z16" s="82"/>
+      <c r="AA16" s="82"/>
+      <c r="AB16" s="82"/>
+      <c r="AC16" s="82"/>
+      <c r="AD16" s="82"/>
       <c r="AE16" s="22"/>
       <c r="AF16" s="22"/>
       <c r="AG16" s="22"/>
@@ -11084,11 +11154,11 @@
       <c r="W17" s="22"/>
       <c r="X17" s="22"/>
       <c r="Y17" s="35"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="60"/>
-      <c r="AB17" s="60"/>
-      <c r="AC17" s="60"/>
-      <c r="AD17" s="60"/>
+      <c r="Z17" s="58"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="58"/>
+      <c r="AC17" s="58"/>
+      <c r="AD17" s="58"/>
       <c r="AE17" s="36"/>
       <c r="AF17" s="22"/>
       <c r="AG17" s="22"/>
@@ -11156,11 +11226,11 @@
       <c r="W18" s="22"/>
       <c r="X18" s="22"/>
       <c r="Y18" s="35"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="60"/>
-      <c r="AB18" s="60"/>
-      <c r="AC18" s="60"/>
-      <c r="AD18" s="60"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="58"/>
+      <c r="AC18" s="58"/>
+      <c r="AD18" s="58"/>
       <c r="AE18" s="22"/>
       <c r="AF18" s="22"/>
       <c r="AG18" s="22"/>
@@ -11226,11 +11296,11 @@
       <c r="W19" s="22"/>
       <c r="X19" s="22"/>
       <c r="Y19" s="35"/>
-      <c r="Z19" s="70"/>
-      <c r="AA19" s="70"/>
-      <c r="AB19" s="70"/>
-      <c r="AC19" s="70"/>
-      <c r="AD19" s="70"/>
+      <c r="Z19" s="68"/>
+      <c r="AA19" s="68"/>
+      <c r="AB19" s="68"/>
+      <c r="AC19" s="68"/>
+      <c r="AD19" s="68"/>
       <c r="AE19" s="22"/>
       <c r="AF19" s="22"/>
       <c r="AG19" s="22"/>
@@ -11296,11 +11366,11 @@
       <c r="W20" s="22"/>
       <c r="X20" s="22"/>
       <c r="Y20" s="35"/>
-      <c r="Z20" s="85"/>
-      <c r="AA20" s="85"/>
-      <c r="AB20" s="85"/>
-      <c r="AC20" s="85"/>
-      <c r="AD20" s="85"/>
+      <c r="Z20" s="82"/>
+      <c r="AA20" s="82"/>
+      <c r="AB20" s="82"/>
+      <c r="AC20" s="82"/>
+      <c r="AD20" s="82"/>
       <c r="AE20" s="22"/>
       <c r="AF20" s="22"/>
       <c r="AG20" s="22"/>
@@ -11366,11 +11436,11 @@
       <c r="W21" s="22"/>
       <c r="X21" s="38"/>
       <c r="Y21" s="35"/>
-      <c r="Z21" s="60"/>
-      <c r="AA21" s="60"/>
-      <c r="AB21" s="60"/>
-      <c r="AC21" s="60"/>
-      <c r="AD21" s="60"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58"/>
+      <c r="AD21" s="58"/>
       <c r="AE21" s="22"/>
       <c r="AF21" s="22"/>
       <c r="AG21" s="22"/>
@@ -12338,52 +12408,52 @@
         <v>366</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="111" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+    <row r="2" spans="1:19" s="108" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="105" t="s">
         <v>361</v>
       </c>
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="106" t="s">
         <v>422</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="105" t="s">
         <v>427</v>
       </c>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="105" t="s">
         <v>428</v>
       </c>
-      <c r="E2" s="108" t="s">
+      <c r="E2" s="105" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="109" t="s">
+      <c r="F2" s="106" t="s">
         <v>429</v>
       </c>
-      <c r="G2" s="108" t="s">
+      <c r="G2" s="105" t="s">
         <v>424</v>
       </c>
-      <c r="H2" s="108" t="s">
+      <c r="H2" s="105" t="s">
         <v>425</v>
       </c>
-      <c r="I2" s="108" t="s">
+      <c r="I2" s="105" t="s">
         <v>426</v>
       </c>
-      <c r="J2" s="108" t="s">
+      <c r="J2" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="108" t="s">
+      <c r="K2" s="105" t="s">
         <v>362</v>
       </c>
-      <c r="L2" s="108" t="s">
+      <c r="L2" s="105" t="s">
         <v>303</v>
       </c>
-      <c r="M2" s="109" t="s">
+      <c r="M2" s="106" t="s">
         <v>172</v>
       </c>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="107"/>
+      <c r="P2" s="107"/>
+      <c r="Q2" s="107"/>
+      <c r="R2" s="107"/>
+      <c r="S2" s="107"/>
     </row>
     <row r="3" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
@@ -13498,46 +13568,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B673FAB6-1E3C-4258-9C8D-D9DBE685A34B}">
   <dimension ref="A1:AK44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="60" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" style="59" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="59" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="59" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="59" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="59" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" style="59" customWidth="1"/>
-    <col min="8" max="8" width="4" style="59" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="58" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" style="59" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" style="59" customWidth="1"/>
-    <col min="12" max="12" width="2.42578125" style="59" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="58" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" style="59" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" style="59" customWidth="1"/>
-    <col min="16" max="16" width="2.7109375" style="59" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="59" customWidth="1"/>
-    <col min="18" max="18" width="5" style="59" customWidth="1"/>
-    <col min="19" max="19" width="2.5703125" style="59" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" style="58" customWidth="1"/>
-    <col min="21" max="21" width="2.28515625" style="60" customWidth="1"/>
-    <col min="22" max="25" width="4.85546875" style="60" customWidth="1"/>
-    <col min="26" max="26" width="10.28515625" style="60" customWidth="1"/>
-    <col min="27" max="27" width="5.140625" style="60" customWidth="1"/>
-    <col min="28" max="29" width="4.7109375" style="60" customWidth="1"/>
-    <col min="30" max="30" width="17.42578125" style="60" customWidth="1"/>
-    <col min="31" max="31" width="5.28515625" style="60" customWidth="1"/>
-    <col min="32" max="32" width="4.42578125" style="60" customWidth="1"/>
-    <col min="33" max="33" width="4.28515625" style="60" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" style="60" customWidth="1"/>
-    <col min="35" max="35" width="7.5703125" style="60" customWidth="1"/>
-    <col min="36" max="36" width="11.85546875" style="60" customWidth="1"/>
-    <col min="37" max="37" width="3.85546875" style="60" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="60"/>
+    <col min="1" max="1" width="1.5703125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" style="57" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="57" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" style="57" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" style="57" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="57" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="4" style="57" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="56" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" style="57" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="57" customWidth="1"/>
+    <col min="12" max="12" width="2.42578125" style="57" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="56" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" style="57" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" style="57" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="57" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="57" customWidth="1"/>
+    <col min="18" max="18" width="5" style="57" customWidth="1"/>
+    <col min="19" max="19" width="2.5703125" style="57" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="56" customWidth="1"/>
+    <col min="21" max="21" width="2.28515625" style="58" customWidth="1"/>
+    <col min="22" max="25" width="4.85546875" style="58" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" style="58" customWidth="1"/>
+    <col min="27" max="27" width="5.140625" style="58" customWidth="1"/>
+    <col min="28" max="29" width="4.7109375" style="58" customWidth="1"/>
+    <col min="30" max="30" width="17.42578125" style="58" customWidth="1"/>
+    <col min="31" max="31" width="5.28515625" style="58" customWidth="1"/>
+    <col min="32" max="32" width="4.42578125" style="58" customWidth="1"/>
+    <col min="33" max="33" width="4.28515625" style="58" customWidth="1"/>
+    <col min="34" max="34" width="6.140625" style="58" customWidth="1"/>
+    <col min="35" max="35" width="7.5703125" style="58" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" style="58" customWidth="1"/>
+    <col min="37" max="37" width="3.85546875" style="58" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -13563,80 +13633,80 @@
       <c r="S1" s="15"/>
       <c r="T1" s="17"/>
     </row>
-    <row r="2" spans="1:37" s="71" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113"/>
-      <c r="B2" s="56" t="s">
+    <row r="2" spans="1:37" s="69" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="110"/>
+      <c r="B2" s="111" t="s">
         <v>363</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="111" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="111" t="s">
         <v>368</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="111" t="s">
         <v>406</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="111" t="s">
         <v>405</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="111" t="s">
         <v>367</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="111" t="s">
         <v>361</v>
       </c>
-      <c r="I2" s="57" t="s">
-        <v>422</v>
-      </c>
-      <c r="J2" s="56" t="s">
-        <v>427</v>
-      </c>
-      <c r="K2" s="56" t="s">
-        <v>428</v>
-      </c>
-      <c r="L2" s="56" t="s">
-        <v>423</v>
-      </c>
-      <c r="M2" s="57" t="s">
-        <v>429</v>
-      </c>
-      <c r="N2" s="56" t="s">
-        <v>424</v>
-      </c>
-      <c r="O2" s="56" t="s">
-        <v>425</v>
-      </c>
-      <c r="P2" s="56" t="s">
-        <v>426</v>
-      </c>
-      <c r="Q2" s="56" t="s">
+      <c r="I2" s="112" t="s">
+        <v>432</v>
+      </c>
+      <c r="J2" s="113" t="s">
+        <v>431</v>
+      </c>
+      <c r="K2" s="113" t="s">
+        <v>436</v>
+      </c>
+      <c r="L2" s="113" t="s">
+        <v>433</v>
+      </c>
+      <c r="M2" s="112" t="s">
+        <v>438</v>
+      </c>
+      <c r="N2" s="113" t="s">
+        <v>434</v>
+      </c>
+      <c r="O2" s="113" t="s">
+        <v>435</v>
+      </c>
+      <c r="P2" s="113" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q2" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="56" t="s">
+      <c r="R2" s="113" t="s">
         <v>362</v>
       </c>
-      <c r="S2" s="56" t="s">
+      <c r="S2" s="111" t="s">
         <v>303</v>
       </c>
-      <c r="T2" s="57" t="s">
+      <c r="T2" s="114" t="s">
         <v>172</v>
       </c>
-      <c r="U2" s="56" t="s">
+      <c r="U2" s="111" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="112">
+      <c r="A3" s="109">
         <v>1</v>
       </c>
       <c r="B3" s="16">
-        <v>0.15179126609969301</v>
+        <v>0.151741535279967</v>
       </c>
       <c r="C3" s="34">
         <v>7.1268826017500304</v>
       </c>
-      <c r="D3" s="96">
+      <c r="D3" s="93">
         <v>0.61999379158845302</v>
       </c>
       <c r="E3" s="15">
@@ -13652,59 +13722,59 @@
         <f t="shared" ref="H3:H11" si="0">(N3-J3)/J3</f>
         <v>5.5214723926380431E-2</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="87" t="s">
         <v>296</v>
       </c>
-      <c r="J3" s="91">
+      <c r="J3" s="88">
         <v>48.9</v>
       </c>
-      <c r="K3" s="91">
+      <c r="K3" s="88">
         <v>3.3</v>
       </c>
-      <c r="L3" s="91">
+      <c r="L3" s="88">
         <v>9</v>
       </c>
-      <c r="M3" s="90" t="s">
+      <c r="M3" s="87" t="s">
         <v>407</v>
       </c>
-      <c r="N3" s="91">
+      <c r="N3" s="88">
         <v>51.6</v>
       </c>
-      <c r="O3" s="91">
+      <c r="O3" s="88">
         <v>5.2</v>
       </c>
-      <c r="P3" s="91">
+      <c r="P3" s="88">
         <v>13</v>
       </c>
-      <c r="Q3" s="91" t="s">
+      <c r="Q3" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="91" t="s">
+      <c r="R3" s="88" t="s">
         <v>359</v>
       </c>
-      <c r="S3" s="91" t="s">
+      <c r="S3" s="88" t="s">
         <v>308</v>
       </c>
-      <c r="T3" s="90" t="s">
+      <c r="T3" s="87" t="s">
         <v>408</v>
       </c>
-      <c r="U3" s="99" t="s">
+      <c r="U3" s="96" t="s">
         <v>420</v>
       </c>
-      <c r="V3" s="99"/>
+      <c r="V3" s="96"/>
       <c r="Z3" s="40"/>
     </row>
-    <row r="4" spans="1:37" s="85" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="112">
+    <row r="4" spans="1:37" s="82" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="109">
         <v>2</v>
       </c>
       <c r="B4" s="50">
-        <v>0.24129939710994899</v>
+        <v>0.23369253545264301</v>
       </c>
       <c r="C4" s="44">
         <v>158840.570149281</v>
       </c>
-      <c r="D4" s="97">
+      <c r="D4" s="94">
         <v>3.5713564070074102E-2</v>
       </c>
       <c r="E4" s="44">
@@ -13720,57 +13790,57 @@
         <f t="shared" si="0"/>
         <v>7.1802543006731492E-3</v>
       </c>
-      <c r="I4" s="92" t="s">
+      <c r="I4" s="89" t="s">
         <v>409</v>
       </c>
-      <c r="J4" s="93">
+      <c r="J4" s="90">
         <v>668500</v>
       </c>
-      <c r="K4" s="93">
+      <c r="K4" s="90">
         <v>106700</v>
       </c>
-      <c r="L4" s="93">
+      <c r="L4" s="90">
         <v>8</v>
       </c>
-      <c r="M4" s="92" t="s">
+      <c r="M4" s="89" t="s">
         <v>410</v>
       </c>
-      <c r="N4" s="93">
+      <c r="N4" s="90">
         <v>673300</v>
       </c>
-      <c r="O4" s="93">
+      <c r="O4" s="90">
         <v>157300</v>
       </c>
-      <c r="P4" s="93">
+      <c r="P4" s="90">
         <v>8</v>
       </c>
-      <c r="Q4" s="93" t="s">
+      <c r="Q4" s="90" t="s">
         <v>353</v>
       </c>
-      <c r="R4" s="93">
+      <c r="R4" s="90">
         <v>0.05</v>
       </c>
-      <c r="S4" s="93" t="s">
+      <c r="S4" s="90" t="s">
         <v>308</v>
       </c>
-      <c r="T4" s="92" t="s">
+      <c r="T4" s="89" t="s">
         <v>411</v>
       </c>
       <c r="U4" s="15"/>
       <c r="V4" s="15"/>
       <c r="Z4" s="44"/>
     </row>
-    <row r="5" spans="1:37" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="112">
+    <row r="5" spans="1:37" s="68" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="109">
         <v>3</v>
       </c>
       <c r="B5" s="51">
-        <v>0.31491948549316001</v>
-      </c>
-      <c r="C5" s="94">
+        <v>0.31705000209038497</v>
+      </c>
+      <c r="C5" s="91">
         <v>115266.14071585301</v>
       </c>
-      <c r="D5" s="98">
+      <c r="D5" s="95">
         <v>5.0486469068246699E-2</v>
       </c>
       <c r="E5" s="53">
@@ -13822,22 +13892,22 @@
       <c r="T5" s="52" t="s">
         <v>293</v>
       </c>
-      <c r="U5" s="99" t="s">
+      <c r="U5" s="96" t="s">
         <v>420</v>
       </c>
-      <c r="Z5" s="94"/>
+      <c r="Z5" s="91"/>
     </row>
     <row r="6" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="112">
+      <c r="A6" s="109">
         <v>4</v>
       </c>
       <c r="B6" s="16">
-        <v>0.31061758132699901</v>
+        <v>0.31147168170758899</v>
       </c>
       <c r="C6" s="28">
         <v>127.23067180345799</v>
       </c>
-      <c r="D6" s="96">
+      <c r="D6" s="93">
         <v>0.91323124927187205</v>
       </c>
       <c r="E6" s="15">
@@ -13889,22 +13959,22 @@
       <c r="T6" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="U6" s="99" t="s">
+      <c r="U6" s="96" t="s">
         <v>420</v>
       </c>
       <c r="Z6" s="28"/>
     </row>
-    <row r="7" spans="1:37" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="112">
+    <row r="7" spans="1:37" s="68" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="109">
         <v>5</v>
       </c>
       <c r="B7" s="51">
-        <v>0.633079824678911</v>
-      </c>
-      <c r="C7" s="95">
+        <v>0.63589532555631401</v>
+      </c>
+      <c r="C7" s="92">
         <v>16.177375293757699</v>
       </c>
-      <c r="D7" s="98">
+      <c r="D7" s="95">
         <v>0.39130715079531098</v>
       </c>
       <c r="E7" s="53">
@@ -13938,7 +14008,7 @@
       <c r="N7" s="53">
         <v>19.399999999999999</v>
       </c>
-      <c r="O7" s="95">
+      <c r="O7" s="92">
         <v>7.15</v>
       </c>
       <c r="P7" s="53">
@@ -13956,157 +14026,157 @@
       <c r="T7" s="52" t="s">
         <v>421</v>
       </c>
-      <c r="U7" s="99" t="s">
+      <c r="U7" s="96" t="s">
         <v>420</v>
       </c>
-      <c r="Z7" s="95"/>
-    </row>
-    <row r="8" spans="1:37" s="85" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="112">
+      <c r="Z7" s="92"/>
+    </row>
+    <row r="8" spans="1:37" s="82" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="109">
         <v>6</v>
       </c>
-      <c r="B8" s="16">
-        <v>1.09857171516531</v>
-      </c>
-      <c r="C8" s="34">
+      <c r="B8" s="50">
+        <v>1.0533902045265899</v>
+      </c>
+      <c r="C8" s="101">
+        <v>34.608572305934999</v>
+      </c>
+      <c r="D8" s="94">
+        <v>0.12847995194645101</v>
+      </c>
+      <c r="E8" s="44">
+        <v>0.744524617045352</v>
+      </c>
+      <c r="F8" s="44">
+        <v>0.63465869131768005</v>
+      </c>
+      <c r="G8" s="44">
+        <v>0.37030064190211498</v>
+      </c>
+      <c r="H8" s="50">
+        <f>(N8-J8)/J8</f>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="I8" s="102" t="s">
+        <v>418</v>
+      </c>
+      <c r="J8" s="103">
+        <v>36</v>
+      </c>
+      <c r="K8" s="103">
+        <v>23</v>
+      </c>
+      <c r="L8" s="103">
+        <v>15</v>
+      </c>
+      <c r="M8" s="102" t="s">
+        <v>419</v>
+      </c>
+      <c r="N8" s="103">
+        <v>41</v>
+      </c>
+      <c r="O8" s="103">
+        <v>50</v>
+      </c>
+      <c r="P8" s="103">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="103" t="s">
+        <v>49</v>
+      </c>
+      <c r="R8" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="S8" s="103" t="s">
+        <v>312</v>
+      </c>
+      <c r="T8" s="102" t="s">
+        <v>313</v>
+      </c>
+      <c r="U8" s="104" t="s">
+        <v>420</v>
+      </c>
+      <c r="Z8" s="115"/>
+    </row>
+    <row r="9" spans="1:37" s="68" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="109">
+        <v>7</v>
+      </c>
+      <c r="B9" s="51">
+        <v>1.13273873352656</v>
+      </c>
+      <c r="C9" s="121">
         <v>0.71020712681328102</v>
       </c>
-      <c r="D8" s="96">
+      <c r="D9" s="95">
         <v>0.25180073430266697</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E9" s="53">
         <v>0.62356527119917304</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F9" s="53">
         <v>1</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G9" s="53">
         <v>0.46608805098768102</v>
       </c>
-      <c r="H8" s="16">
-        <f t="shared" si="0"/>
+      <c r="H9" s="51">
+        <f>(N9-J9)/J9</f>
         <v>-0.13464235624123419</v>
       </c>
-      <c r="I8" s="92" t="s">
+      <c r="I9" s="98" t="s">
         <v>257</v>
       </c>
-      <c r="J8" s="93">
+      <c r="J9" s="99">
         <v>0.71299999999999997</v>
       </c>
-      <c r="K8" s="93">
+      <c r="K9" s="99">
         <v>0.29699999999999999</v>
       </c>
-      <c r="L8" s="93">
+      <c r="L9" s="99">
         <v>8</v>
       </c>
-      <c r="M8" s="92" t="s">
+      <c r="M9" s="98" t="s">
         <v>300</v>
       </c>
-      <c r="N8" s="93">
+      <c r="N9" s="99">
         <v>0.61699999999999999</v>
       </c>
-      <c r="O8" s="93">
+      <c r="O9" s="99">
         <v>0.45</v>
       </c>
-      <c r="P8" s="93">
+      <c r="P9" s="99">
         <v>8</v>
       </c>
-      <c r="Q8" s="93" t="s">
+      <c r="Q9" s="99" t="s">
         <v>412</v>
       </c>
-      <c r="R8" s="93" t="s">
+      <c r="R9" s="99" t="s">
         <v>356</v>
       </c>
-      <c r="S8" s="93" t="s">
+      <c r="S9" s="99" t="s">
         <v>309</v>
       </c>
-      <c r="T8" s="92" t="s">
+      <c r="T9" s="98" t="s">
         <v>301</v>
       </c>
-      <c r="U8" s="99" t="s">
+      <c r="U9" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="Z8" s="34"/>
-    </row>
-    <row r="9" spans="1:37" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="112">
-        <v>7</v>
-      </c>
-      <c r="B9" s="51">
-        <v>1.06146056606671</v>
-      </c>
-      <c r="C9" s="94">
-        <v>34.608572305934999</v>
-      </c>
-      <c r="D9" s="98">
-        <v>0.12847995194645101</v>
-      </c>
-      <c r="E9" s="53">
-        <v>0.744524617045352</v>
-      </c>
-      <c r="F9" s="53">
-        <v>0.63465869131768005</v>
-      </c>
-      <c r="G9" s="53">
-        <v>0.37030064190211498</v>
-      </c>
-      <c r="H9" s="51">
-        <f t="shared" si="0"/>
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="I9" s="101" t="s">
-        <v>418</v>
-      </c>
-      <c r="J9" s="102">
-        <v>36</v>
-      </c>
-      <c r="K9" s="102">
-        <v>23</v>
-      </c>
-      <c r="L9" s="102">
-        <v>15</v>
-      </c>
-      <c r="M9" s="101" t="s">
-        <v>419</v>
-      </c>
-      <c r="N9" s="102">
-        <v>41</v>
-      </c>
-      <c r="O9" s="102">
-        <v>50</v>
-      </c>
-      <c r="P9" s="102">
-        <v>13</v>
-      </c>
-      <c r="Q9" s="102" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" s="102">
-        <v>0.05</v>
-      </c>
-      <c r="S9" s="102" t="s">
-        <v>312</v>
-      </c>
-      <c r="T9" s="101" t="s">
-        <v>313</v>
-      </c>
-      <c r="U9" s="103" t="s">
-        <v>420</v>
-      </c>
-      <c r="X9" s="94"/>
-      <c r="Z9" s="95"/>
-    </row>
-    <row r="10" spans="1:37" s="85" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="112">
+      <c r="X9" s="91"/>
+      <c r="Z9" s="92"/>
+    </row>
+    <row r="10" spans="1:37" s="82" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="109">
         <v>8</v>
       </c>
       <c r="B10" s="50">
-        <v>3.99759047989915</v>
-      </c>
-      <c r="C10" s="94">
+        <v>3.80465684953018</v>
+      </c>
+      <c r="C10" s="91">
         <v>749292.30353048595</v>
       </c>
-      <c r="D10" s="97">
+      <c r="D10" s="94">
         <v>3.9523876652813497E-2</v>
       </c>
       <c r="E10" s="44">
@@ -14122,58 +14192,58 @@
         <f t="shared" si="0"/>
         <v>1.8032205992361904E-2</v>
       </c>
-      <c r="I10" s="105" t="s">
+      <c r="I10" s="102" t="s">
         <v>291</v>
       </c>
-      <c r="J10" s="106">
+      <c r="J10" s="103">
         <v>304788</v>
       </c>
-      <c r="K10" s="106">
+      <c r="K10" s="103">
         <v>113425</v>
       </c>
-      <c r="L10" s="106">
+      <c r="L10" s="103">
         <v>4</v>
       </c>
-      <c r="M10" s="105" t="s">
+      <c r="M10" s="102" t="s">
         <v>341</v>
       </c>
-      <c r="N10" s="106">
+      <c r="N10" s="103">
         <v>310284</v>
       </c>
-      <c r="O10" s="106">
+      <c r="O10" s="103">
         <v>160647</v>
       </c>
-      <c r="P10" s="106">
+      <c r="P10" s="103">
         <v>3</v>
       </c>
-      <c r="Q10" s="106" t="s">
+      <c r="Q10" s="103" t="s">
         <v>413</v>
       </c>
-      <c r="R10" s="106" t="s">
+      <c r="R10" s="103" t="s">
         <v>359</v>
       </c>
-      <c r="S10" s="106" t="s">
+      <c r="S10" s="103" t="s">
         <v>332</v>
       </c>
-      <c r="T10" s="105" t="s">
+      <c r="T10" s="102" t="s">
         <v>339</v>
       </c>
-      <c r="U10" s="107" t="s">
+      <c r="U10" s="104" t="s">
         <v>420</v>
       </c>
-      <c r="Z10" s="104"/>
-    </row>
-    <row r="11" spans="1:37" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="112">
+      <c r="Z10" s="101"/>
+    </row>
+    <row r="11" spans="1:37" s="68" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="109">
         <v>9</v>
       </c>
       <c r="B11" s="51">
-        <v>4.8342169763688796</v>
-      </c>
-      <c r="C11" s="94">
+        <v>4.8920217179999002</v>
+      </c>
+      <c r="C11" s="91">
         <v>17727.333292926902</v>
       </c>
-      <c r="D11" s="98">
+      <c r="D11" s="95">
         <v>0.57883864704215804</v>
       </c>
       <c r="E11" s="53">
@@ -14195,7 +14265,7 @@
       <c r="J11" s="53">
         <v>9956</v>
       </c>
-      <c r="K11" s="94">
+      <c r="K11" s="91">
         <f>(12545-J11)*SQRT(L11)</f>
         <v>11578.359987493912</v>
       </c>
@@ -14208,7 +14278,7 @@
       <c r="N11" s="53">
         <v>17196</v>
       </c>
-      <c r="O11" s="94">
+      <c r="O11" s="91">
         <f>(20348-N11)*SQRT(P11)</f>
         <v>13372.803445799986</v>
       </c>
@@ -14227,1596 +14297,1593 @@
       <c r="T11" s="52" t="s">
         <v>399</v>
       </c>
-      <c r="U11" s="99" t="s">
+      <c r="U11" s="96" t="s">
         <v>420</v>
       </c>
-      <c r="Z11" s="94"/>
-    </row>
-    <row r="12" spans="1:37" s="85" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="64"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="66"/>
-      <c r="T12" s="65"/>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="C14" s="72"/>
+      <c r="Z11" s="91"/>
+    </row>
+    <row r="12" spans="1:37" s="82" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="62"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="64"/>
+      <c r="S12" s="64"/>
+      <c r="T12" s="63"/>
     </row>
     <row r="15" spans="1:37" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V15" s="73"/>
-      <c r="W15" s="73"/>
-      <c r="X15" s="73"/>
-      <c r="Y15" s="73"/>
-      <c r="Z15" s="73"/>
-      <c r="AA15" s="73"/>
-      <c r="AB15" s="73"/>
-      <c r="AC15" s="73"/>
-      <c r="AD15" s="73"/>
-      <c r="AE15" s="73"/>
-      <c r="AF15" s="73"/>
-      <c r="AG15" s="73"/>
-      <c r="AH15" s="73"/>
-      <c r="AI15" s="73"/>
-      <c r="AJ15" s="73"/>
-      <c r="AK15" s="73"/>
+      <c r="V15" s="70"/>
+      <c r="W15" s="70"/>
+      <c r="X15" s="70"/>
+      <c r="Y15" s="70"/>
+      <c r="Z15" s="70"/>
+      <c r="AA15" s="70"/>
+      <c r="AB15" s="70"/>
+      <c r="AC15" s="70"/>
+      <c r="AD15" s="70"/>
+      <c r="AE15" s="70"/>
+      <c r="AF15" s="70"/>
+      <c r="AG15" s="70"/>
+      <c r="AH15" s="70"/>
+      <c r="AI15" s="70"/>
+      <c r="AJ15" s="70"/>
+      <c r="AK15" s="70"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="73"/>
-      <c r="Y16" s="73"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="73"/>
-      <c r="AB16" s="73"/>
-      <c r="AC16" s="73"/>
-      <c r="AD16" s="73"/>
-      <c r="AE16" s="73"/>
-      <c r="AF16" s="73"/>
-      <c r="AG16" s="73"/>
-      <c r="AH16" s="73"/>
-      <c r="AI16" s="73"/>
-      <c r="AJ16" s="73"/>
-      <c r="AK16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="V16" s="70"/>
+      <c r="W16" s="70"/>
+      <c r="X16" s="70"/>
+      <c r="Y16" s="70"/>
+      <c r="Z16" s="70"/>
+      <c r="AA16" s="70"/>
+      <c r="AB16" s="70"/>
+      <c r="AC16" s="70"/>
+      <c r="AD16" s="70"/>
+      <c r="AE16" s="70"/>
+      <c r="AF16" s="70"/>
+      <c r="AG16" s="70"/>
+      <c r="AH16" s="70"/>
+      <c r="AI16" s="70"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
     </row>
     <row r="17" spans="2:37" x14ac:dyDescent="0.15">
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="V17" s="73"/>
-      <c r="W17" s="73"/>
-      <c r="X17" s="73"/>
-      <c r="Y17" s="73"/>
-      <c r="Z17" s="73"/>
-      <c r="AA17" s="73"/>
-      <c r="AB17" s="73"/>
-      <c r="AC17" s="73"/>
-      <c r="AD17" s="73"/>
-      <c r="AE17" s="73"/>
-      <c r="AF17" s="73"/>
-      <c r="AG17" s="73"/>
-      <c r="AH17" s="73"/>
-      <c r="AI17" s="73"/>
-      <c r="AJ17" s="73"/>
-      <c r="AK17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="V17" s="70"/>
+      <c r="W17" s="70"/>
+      <c r="X17" s="70"/>
+      <c r="Y17" s="70"/>
+      <c r="Z17" s="70"/>
+      <c r="AA17" s="70"/>
+      <c r="AB17" s="70"/>
+      <c r="AC17" s="70"/>
+      <c r="AD17" s="70"/>
+      <c r="AE17" s="70"/>
+      <c r="AF17" s="70"/>
+      <c r="AG17" s="70"/>
+      <c r="AH17" s="70"/>
+      <c r="AI17" s="70"/>
+      <c r="AJ17" s="70"/>
+      <c r="AK17" s="70"/>
     </row>
     <row r="18" spans="2:37" x14ac:dyDescent="0.15">
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="U18" s="71"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74"/>
-      <c r="X18" s="74"/>
-      <c r="Y18" s="74"/>
-      <c r="Z18" s="74"/>
-      <c r="AA18" s="73"/>
-      <c r="AB18" s="73"/>
-      <c r="AC18" s="73"/>
-      <c r="AD18" s="73"/>
-      <c r="AE18" s="73"/>
-      <c r="AF18" s="73"/>
-      <c r="AG18" s="73"/>
-      <c r="AH18" s="73"/>
-      <c r="AI18" s="73"/>
-      <c r="AJ18" s="73"/>
-      <c r="AK18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="U18" s="69"/>
+      <c r="V18" s="71"/>
+      <c r="W18" s="71"/>
+      <c r="X18" s="71"/>
+      <c r="Y18" s="71"/>
+      <c r="Z18" s="71"/>
+      <c r="AA18" s="70"/>
+      <c r="AB18" s="70"/>
+      <c r="AC18" s="70"/>
+      <c r="AD18" s="70"/>
+      <c r="AE18" s="70"/>
+      <c r="AF18" s="70"/>
+      <c r="AG18" s="70"/>
+      <c r="AH18" s="70"/>
+      <c r="AI18" s="70"/>
+      <c r="AJ18" s="70"/>
+      <c r="AK18" s="70"/>
     </row>
     <row r="19" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="72" t="s">
         <v>377</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="D19" s="75" t="s">
+      <c r="D19" s="72" t="s">
         <v>379</v>
       </c>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="78" t="s">
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="75" t="s">
         <v>168</v>
       </c>
-      <c r="J19" s="75" t="s">
+      <c r="J19" s="72" t="s">
         <v>380</v>
       </c>
-      <c r="K19" s="75" t="s">
+      <c r="K19" s="72" t="s">
         <v>381</v>
       </c>
-      <c r="L19" s="75" t="s">
+      <c r="L19" s="72" t="s">
         <v>382</v>
       </c>
-      <c r="M19" s="78" t="s">
+      <c r="M19" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="N19" s="75" t="s">
+      <c r="N19" s="72" t="s">
         <v>383</v>
       </c>
-      <c r="O19" s="75" t="s">
+      <c r="O19" s="72" t="s">
         <v>384</v>
       </c>
-      <c r="P19" s="75" t="s">
+      <c r="P19" s="72" t="s">
         <v>385</v>
       </c>
-      <c r="Q19" s="75" t="s">
+      <c r="Q19" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="R19" s="75" t="s">
+      <c r="R19" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="S19" s="75" t="s">
+      <c r="S19" s="72" t="s">
         <v>303</v>
       </c>
-      <c r="T19" s="78" t="s">
+      <c r="T19" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="V19" s="73"/>
-      <c r="W19" s="76"/>
-      <c r="X19" s="76"/>
-      <c r="Y19" s="76"/>
-      <c r="Z19" s="77"/>
-      <c r="AA19" s="76"/>
-      <c r="AB19" s="76"/>
-      <c r="AC19" s="76"/>
-      <c r="AD19" s="77"/>
-      <c r="AE19" s="76"/>
-      <c r="AF19" s="76"/>
-      <c r="AG19" s="76"/>
-      <c r="AH19" s="76"/>
-      <c r="AI19" s="76"/>
-      <c r="AJ19" s="77"/>
-      <c r="AK19" s="73"/>
+      <c r="V19" s="70"/>
+      <c r="W19" s="73"/>
+      <c r="X19" s="73"/>
+      <c r="Y19" s="73"/>
+      <c r="Z19" s="74"/>
+      <c r="AA19" s="73"/>
+      <c r="AB19" s="73"/>
+      <c r="AC19" s="73"/>
+      <c r="AD19" s="74"/>
+      <c r="AE19" s="73"/>
+      <c r="AF19" s="73"/>
+      <c r="AG19" s="73"/>
+      <c r="AH19" s="73"/>
+      <c r="AI19" s="73"/>
+      <c r="AJ19" s="74"/>
+      <c r="AK19" s="70"/>
     </row>
     <row r="20" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="61">
+      <c r="B20" s="59">
         <v>0.22021648333308816</v>
       </c>
-      <c r="C20" s="67">
+      <c r="C20" s="65">
         <v>0.15701435261649185</v>
       </c>
-      <c r="D20" s="59">
+      <c r="D20" s="57">
         <v>-1.542776998597477E-2</v>
       </c>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="58" t="s">
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="56" t="s">
         <v>358</v>
       </c>
-      <c r="J20" s="59">
+      <c r="J20" s="57">
         <v>0.71299999999999997</v>
       </c>
-      <c r="K20" s="62">
+      <c r="K20" s="60">
         <f>0.105*SQRT(L20)</f>
         <v>0.29698484809834996</v>
       </c>
-      <c r="L20" s="59">
+      <c r="L20" s="57">
         <v>8</v>
       </c>
-      <c r="M20" s="58" t="s">
+      <c r="M20" s="56" t="s">
         <v>300</v>
       </c>
-      <c r="N20" s="59">
+      <c r="N20" s="57">
         <v>0.61699999999999999</v>
       </c>
-      <c r="O20" s="62">
+      <c r="O20" s="60">
         <f>0.159*SQRT(P20)</f>
         <v>0.44971991283464424</v>
       </c>
-      <c r="P20" s="59">
+      <c r="P20" s="57">
         <v>8</v>
       </c>
-      <c r="Q20" s="59" t="s">
+      <c r="Q20" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="R20" s="59">
+      <c r="R20" s="57">
         <v>7</v>
       </c>
-      <c r="S20" s="59" t="s">
+      <c r="S20" s="57" t="s">
         <v>309</v>
       </c>
-      <c r="T20" s="58" t="s">
+      <c r="T20" s="56" t="s">
         <v>301</v>
       </c>
-      <c r="V20" s="76"/>
-      <c r="W20" s="76"/>
-      <c r="X20" s="76"/>
-      <c r="Y20" s="79"/>
-      <c r="Z20" s="80"/>
-      <c r="AA20" s="81"/>
-      <c r="AB20" s="82"/>
-      <c r="AC20" s="76"/>
-      <c r="AD20" s="80"/>
-      <c r="AE20" s="81"/>
-      <c r="AF20" s="76"/>
-      <c r="AG20" s="76"/>
-      <c r="AH20" s="76"/>
-      <c r="AI20" s="76"/>
-      <c r="AJ20" s="83"/>
-      <c r="AK20" s="73"/>
+      <c r="V20" s="73"/>
+      <c r="W20" s="73"/>
+      <c r="X20" s="73"/>
+      <c r="Y20" s="76"/>
+      <c r="Z20" s="77"/>
+      <c r="AA20" s="78"/>
+      <c r="AB20" s="79"/>
+      <c r="AC20" s="73"/>
+      <c r="AD20" s="77"/>
+      <c r="AE20" s="78"/>
+      <c r="AF20" s="73"/>
+      <c r="AG20" s="73"/>
+      <c r="AH20" s="73"/>
+      <c r="AI20" s="73"/>
+      <c r="AJ20" s="80"/>
+      <c r="AK20" s="70"/>
     </row>
     <row r="21" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="61">
+      <c r="B21" s="59">
         <f t="shared" ref="B21:B38" si="1">C21/J21</f>
         <v>0.30233492648200283</v>
       </c>
-      <c r="C21" s="63">
+      <c r="C21" s="61">
         <f t="shared" ref="C21:C38" si="2">ABS(N21-J21) + ABS(_xlfn.NORM.S.INV(1-(0.05/R21)/2))*SQRT(K21^2/L21+O21^2/P21)</f>
         <v>110561.76626998305</v>
       </c>
-      <c r="D21" s="61">
+      <c r="D21" s="59">
         <f t="shared" ref="D21:D38" si="3">-(J21-N21)/J21</f>
         <v>-1.9669504201611735E-2</v>
       </c>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="58" t="s">
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="J21" s="59">
+      <c r="J21" s="57">
         <v>365693</v>
       </c>
-      <c r="K21" s="59">
+      <c r="K21" s="57">
         <v>125513</v>
       </c>
-      <c r="L21" s="59">
+      <c r="L21" s="57">
         <v>14</v>
       </c>
-      <c r="M21" s="58" t="s">
+      <c r="M21" s="56" t="s">
         <v>292</v>
       </c>
-      <c r="N21" s="59">
+      <c r="N21" s="57">
         <v>358500</v>
       </c>
-      <c r="O21" s="59">
+      <c r="O21" s="57">
         <v>157620</v>
       </c>
-      <c r="P21" s="59">
+      <c r="P21" s="57">
         <v>15</v>
       </c>
-      <c r="Q21" s="59" t="s">
+      <c r="Q21" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R21" s="59">
+      <c r="R21" s="57">
         <v>1</v>
       </c>
-      <c r="S21" s="59" t="s">
+      <c r="S21" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T21" s="58" t="s">
+      <c r="T21" s="56" t="s">
         <v>293</v>
       </c>
-      <c r="V21" s="76"/>
-      <c r="W21" s="76"/>
-      <c r="X21" s="76"/>
-      <c r="Y21" s="79"/>
-      <c r="Z21" s="77"/>
-      <c r="AA21" s="76"/>
-      <c r="AB21" s="76"/>
-      <c r="AC21" s="76"/>
-      <c r="AD21" s="77"/>
-      <c r="AE21" s="76"/>
-      <c r="AF21" s="76"/>
-      <c r="AG21" s="76"/>
-      <c r="AH21" s="76"/>
-      <c r="AI21" s="76"/>
-      <c r="AJ21" s="77"/>
-      <c r="AK21" s="73"/>
+      <c r="V21" s="73"/>
+      <c r="W21" s="73"/>
+      <c r="X21" s="73"/>
+      <c r="Y21" s="76"/>
+      <c r="Z21" s="74"/>
+      <c r="AA21" s="73"/>
+      <c r="AB21" s="73"/>
+      <c r="AC21" s="73"/>
+      <c r="AD21" s="74"/>
+      <c r="AE21" s="73"/>
+      <c r="AF21" s="73"/>
+      <c r="AG21" s="73"/>
+      <c r="AH21" s="73"/>
+      <c r="AI21" s="73"/>
+      <c r="AJ21" s="74"/>
+      <c r="AK21" s="70"/>
     </row>
     <row r="22" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="61">
+      <c r="B22" s="59">
         <f t="shared" si="1"/>
         <v>0.33187378676985985</v>
       </c>
-      <c r="C22" s="67">
+      <c r="C22" s="65">
         <f t="shared" si="2"/>
         <v>8.5955310773393698</v>
       </c>
-      <c r="D22" s="61">
+      <c r="D22" s="59">
         <f t="shared" si="3"/>
         <v>-0.1274131274131273</v>
       </c>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="58" t="s">
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="56" t="s">
         <v>371</v>
       </c>
-      <c r="J22" s="59">
+      <c r="J22" s="57">
         <v>25.9</v>
       </c>
-      <c r="K22" s="59">
+      <c r="K22" s="57">
         <f>1.7*SQRT(L22)</f>
         <v>6.8</v>
       </c>
-      <c r="L22" s="59">
+      <c r="L22" s="57">
         <v>16</v>
       </c>
-      <c r="M22" s="58" t="s">
+      <c r="M22" s="56" t="s">
         <v>372</v>
       </c>
-      <c r="N22" s="59">
+      <c r="N22" s="57">
         <v>22.6</v>
       </c>
-      <c r="O22" s="68">
+      <c r="O22" s="66">
         <f>2.1*SQRT(P22)</f>
         <v>8.1332650270355753</v>
       </c>
-      <c r="P22" s="59">
+      <c r="P22" s="57">
         <v>15</v>
       </c>
-      <c r="Q22" s="59" t="s">
+      <c r="Q22" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="R22" s="59">
+      <c r="R22" s="57">
         <v>1</v>
       </c>
-      <c r="S22" s="59" t="s">
+      <c r="S22" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T22" s="58" t="s">
+      <c r="T22" s="56" t="s">
         <v>289</v>
       </c>
-      <c r="V22" s="76"/>
-      <c r="W22" s="76"/>
-      <c r="X22" s="76"/>
-      <c r="Y22" s="79"/>
-      <c r="Z22" s="77"/>
-      <c r="AA22" s="76"/>
-      <c r="AB22" s="76"/>
-      <c r="AC22" s="76"/>
-      <c r="AD22" s="77"/>
-      <c r="AE22" s="76"/>
-      <c r="AF22" s="76"/>
-      <c r="AG22" s="76"/>
-      <c r="AH22" s="76"/>
-      <c r="AI22" s="76"/>
-      <c r="AJ22" s="77"/>
-      <c r="AK22" s="73"/>
+      <c r="V22" s="73"/>
+      <c r="W22" s="73"/>
+      <c r="X22" s="73"/>
+      <c r="Y22" s="76"/>
+      <c r="Z22" s="74"/>
+      <c r="AA22" s="73"/>
+      <c r="AB22" s="73"/>
+      <c r="AC22" s="73"/>
+      <c r="AD22" s="74"/>
+      <c r="AE22" s="73"/>
+      <c r="AF22" s="73"/>
+      <c r="AG22" s="73"/>
+      <c r="AH22" s="73"/>
+      <c r="AI22" s="73"/>
+      <c r="AJ22" s="74"/>
+      <c r="AK22" s="70"/>
     </row>
     <row r="23" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="61">
+      <c r="B23" s="59">
         <f t="shared" si="1"/>
         <v>0.3351756133312177</v>
       </c>
-      <c r="C23" s="63">
+      <c r="C23" s="61">
         <f t="shared" si="2"/>
         <v>8.7145659466116605</v>
       </c>
-      <c r="D23" s="61">
+      <c r="D23" s="59">
         <f t="shared" si="3"/>
         <v>4.2307692307692366E-2</v>
       </c>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="58" t="s">
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="56" t="s">
         <v>283</v>
       </c>
-      <c r="J23" s="59">
+      <c r="J23" s="57">
         <v>26</v>
       </c>
-      <c r="K23" s="68">
+      <c r="K23" s="66">
         <f>(28.3-J23)*SQRT(L23)</f>
         <v>6.5053823869162395</v>
       </c>
-      <c r="L23" s="59">
+      <c r="L23" s="57">
         <v>8</v>
       </c>
-      <c r="M23" s="58" t="s">
+      <c r="M23" s="56" t="s">
         <v>284</v>
       </c>
-      <c r="N23" s="59">
+      <c r="N23" s="57">
         <v>27.1</v>
       </c>
-      <c r="O23" s="68">
+      <c r="O23" s="66">
         <f>(28.3-N23)*SQRT(P23)</f>
         <v>3.3941125496954263</v>
       </c>
-      <c r="P23" s="59">
+      <c r="P23" s="57">
         <v>8</v>
       </c>
-      <c r="Q23" s="59" t="s">
+      <c r="Q23" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="R23" s="59">
+      <c r="R23" s="57">
         <v>15</v>
       </c>
-      <c r="S23" s="59" t="s">
+      <c r="S23" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T23" s="58" t="s">
+      <c r="T23" s="56" t="s">
         <v>285</v>
       </c>
-      <c r="V23" s="76"/>
-      <c r="W23" s="76"/>
-      <c r="X23" s="84"/>
-      <c r="Y23" s="79"/>
-      <c r="Z23" s="77"/>
-      <c r="AA23" s="76"/>
-      <c r="AB23" s="76"/>
-      <c r="AC23" s="76"/>
-      <c r="AD23" s="77"/>
-      <c r="AE23" s="76"/>
-      <c r="AF23" s="76"/>
-      <c r="AG23" s="76"/>
-      <c r="AH23" s="76"/>
-      <c r="AI23" s="76"/>
-      <c r="AJ23" s="77"/>
-      <c r="AK23" s="73"/>
+      <c r="V23" s="73"/>
+      <c r="W23" s="73"/>
+      <c r="X23" s="81"/>
+      <c r="Y23" s="76"/>
+      <c r="Z23" s="74"/>
+      <c r="AA23" s="73"/>
+      <c r="AB23" s="73"/>
+      <c r="AC23" s="73"/>
+      <c r="AD23" s="74"/>
+      <c r="AE23" s="73"/>
+      <c r="AF23" s="73"/>
+      <c r="AG23" s="73"/>
+      <c r="AH23" s="73"/>
+      <c r="AI23" s="73"/>
+      <c r="AJ23" s="74"/>
+      <c r="AK23" s="70"/>
     </row>
     <row r="24" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="61">
+      <c r="B24" s="59">
         <f t="shared" si="1"/>
         <v>0.36468210626768915</v>
       </c>
-      <c r="C24" s="68">
+      <c r="C24" s="66">
         <f t="shared" si="2"/>
         <v>131.28555825636809</v>
       </c>
-      <c r="D24" s="61">
+      <c r="D24" s="59">
         <f t="shared" si="3"/>
         <v>-0.18055555555555555</v>
       </c>
-      <c r="I24" s="58" t="s">
+      <c r="I24" s="56" t="s">
         <v>373</v>
       </c>
-      <c r="J24" s="69">
+      <c r="J24" s="67">
         <v>360</v>
       </c>
-      <c r="K24" s="63">
+      <c r="K24" s="61">
         <v>94</v>
       </c>
-      <c r="L24" s="59">
+      <c r="L24" s="57">
         <v>9</v>
       </c>
-      <c r="M24" s="58" t="s">
+      <c r="M24" s="56" t="s">
         <v>374</v>
       </c>
-      <c r="N24" s="59">
+      <c r="N24" s="57">
         <v>295</v>
       </c>
-      <c r="O24" s="68">
+      <c r="O24" s="66">
         <v>36</v>
       </c>
-      <c r="P24" s="59">
+      <c r="P24" s="57">
         <v>8</v>
       </c>
-      <c r="Q24" s="59" t="s">
+      <c r="Q24" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="R24" s="59">
+      <c r="R24" s="57">
         <v>1</v>
       </c>
-      <c r="S24" s="59" t="s">
+      <c r="S24" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T24" s="58" t="s">
+      <c r="T24" s="56" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="25" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="61">
+      <c r="B25" s="59">
         <f t="shared" si="1"/>
         <v>0.38375612642394952</v>
       </c>
-      <c r="C25" s="63">
+      <c r="C25" s="61">
         <f t="shared" si="2"/>
         <v>127779.27741538247</v>
       </c>
-      <c r="D25" s="61">
+      <c r="D25" s="59">
         <f t="shared" si="3"/>
         <v>4.5589692765113973E-2</v>
       </c>
-      <c r="I25" s="58" t="s">
+      <c r="I25" s="56" t="s">
         <v>386</v>
       </c>
-      <c r="J25" s="59">
+      <c r="J25" s="57">
         <v>332970</v>
       </c>
-      <c r="K25" s="63">
+      <c r="K25" s="61">
         <f>(357910-J25)*SQRT(L25)</f>
         <v>70540.972491169989</v>
       </c>
-      <c r="L25" s="59">
+      <c r="L25" s="57">
         <v>8</v>
       </c>
-      <c r="M25" s="58" t="s">
+      <c r="M25" s="56" t="s">
         <v>387</v>
       </c>
-      <c r="N25" s="59">
+      <c r="N25" s="57">
         <v>348150</v>
       </c>
-      <c r="O25" s="59">
+      <c r="O25" s="57">
         <f>(378520-N25)*SQRT(P25)</f>
         <v>74391.003488325106</v>
       </c>
-      <c r="P25" s="59">
+      <c r="P25" s="57">
         <v>6</v>
       </c>
-      <c r="Q25" s="59" t="s">
+      <c r="Q25" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R25" s="59">
+      <c r="R25" s="57">
         <v>12</v>
       </c>
-      <c r="S25" s="59" t="s">
+      <c r="S25" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T25" s="58" t="s">
+      <c r="T25" s="56" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="2:37" s="59" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="61">
+    <row r="26" spans="2:37" s="57" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="59">
         <f t="shared" si="1"/>
         <v>0.43866397912473509</v>
       </c>
-      <c r="C26" s="63">
+      <c r="C26" s="61">
         <f t="shared" si="2"/>
         <v>147.87362736294821</v>
       </c>
-      <c r="D26" s="61">
+      <c r="D26" s="59">
         <f t="shared" si="3"/>
         <v>1.0382675763868287E-2</v>
       </c>
-      <c r="I26" s="58" t="s">
+      <c r="I26" s="56" t="s">
         <v>283</v>
       </c>
-      <c r="J26" s="59">
+      <c r="J26" s="57">
         <v>337.1</v>
       </c>
-      <c r="K26" s="68">
+      <c r="K26" s="66">
         <f>(379.1-J26)*SQRT(L26)</f>
         <v>118.79393923933999</v>
       </c>
-      <c r="L26" s="59">
+      <c r="L26" s="57">
         <v>8</v>
       </c>
-      <c r="M26" s="58" t="s">
+      <c r="M26" s="56" t="s">
         <v>284</v>
       </c>
-      <c r="N26" s="59">
+      <c r="N26" s="57">
         <v>340.6</v>
       </c>
-      <c r="O26" s="68">
+      <c r="O26" s="66">
         <f>(366.2-340.6)*SQRT(P26)</f>
         <v>72.40773439350238</v>
       </c>
-      <c r="P26" s="59">
+      <c r="P26" s="57">
         <v>8</v>
       </c>
-      <c r="Q26" s="59" t="s">
+      <c r="Q26" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R26" s="59">
+      <c r="R26" s="57">
         <v>15</v>
       </c>
-      <c r="S26" s="59" t="s">
+      <c r="S26" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T26" s="58" t="s">
+      <c r="T26" s="56" t="s">
         <v>286</v>
       </c>
-      <c r="U26" s="60"/>
-      <c r="V26" s="60"/>
-      <c r="W26" s="60"/>
-      <c r="X26" s="60"/>
-      <c r="Y26" s="60"/>
-      <c r="Z26" s="60"/>
-      <c r="AA26" s="60"/>
-      <c r="AB26" s="60"/>
-      <c r="AC26" s="60"/>
-      <c r="AD26" s="60"/>
-      <c r="AE26" s="60"/>
-      <c r="AF26" s="60"/>
-      <c r="AG26" s="60"/>
-      <c r="AH26" s="60"/>
-      <c r="AI26" s="60"/>
-      <c r="AJ26" s="60"/>
-      <c r="AK26" s="60"/>
-    </row>
-    <row r="27" spans="2:37" s="59" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="61">
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="58"/>
+      <c r="Y26" s="58"/>
+      <c r="Z26" s="58"/>
+      <c r="AA26" s="58"/>
+      <c r="AB26" s="58"/>
+      <c r="AC26" s="58"/>
+      <c r="AD26" s="58"/>
+      <c r="AE26" s="58"/>
+      <c r="AF26" s="58"/>
+      <c r="AG26" s="58"/>
+      <c r="AH26" s="58"/>
+      <c r="AI26" s="58"/>
+      <c r="AJ26" s="58"/>
+      <c r="AK26" s="58"/>
+    </row>
+    <row r="27" spans="2:37" s="57" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="59">
         <f t="shared" si="1"/>
         <v>0.54447029123354107</v>
       </c>
-      <c r="C27" s="63">
+      <c r="C27" s="61">
         <f t="shared" si="2"/>
         <v>65064.199802408162</v>
       </c>
-      <c r="D27" s="61">
+      <c r="D27" s="59">
         <f t="shared" si="3"/>
         <v>-7.364016736401674E-2</v>
       </c>
-      <c r="I27" s="58" t="s">
+      <c r="I27" s="56" t="s">
         <v>388</v>
       </c>
-      <c r="J27" s="59">
+      <c r="J27" s="57">
         <v>119500</v>
       </c>
-      <c r="K27" s="59">
+      <c r="K27" s="57">
         <f>(135500-J27)*SQRT(L27)</f>
         <v>50596.442562694072</v>
       </c>
-      <c r="L27" s="59">
+      <c r="L27" s="57">
         <v>10</v>
       </c>
-      <c r="M27" s="58" t="s">
+      <c r="M27" s="56" t="s">
         <v>389</v>
       </c>
-      <c r="N27" s="59">
+      <c r="N27" s="57">
         <v>110700</v>
       </c>
-      <c r="O27" s="59">
+      <c r="O27" s="57">
         <f>(124800-N27)*SQRT(P27)</f>
         <v>66134.862213510365</v>
       </c>
-      <c r="P27" s="59">
+      <c r="P27" s="57">
         <v>22</v>
       </c>
-      <c r="Q27" s="59" t="s">
+      <c r="Q27" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R27" s="59">
+      <c r="R27" s="57">
         <v>6</v>
       </c>
-      <c r="S27" s="59" t="s">
+      <c r="S27" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T27" s="58" t="s">
+      <c r="T27" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="U27" s="60"/>
-      <c r="V27" s="60"/>
-      <c r="W27" s="60"/>
-      <c r="X27" s="60"/>
-      <c r="Y27" s="60"/>
-      <c r="Z27" s="60"/>
-      <c r="AA27" s="60"/>
-      <c r="AB27" s="60"/>
-      <c r="AC27" s="60"/>
-      <c r="AD27" s="60"/>
-      <c r="AE27" s="60"/>
-      <c r="AF27" s="60"/>
-      <c r="AG27" s="60"/>
-      <c r="AH27" s="60"/>
-      <c r="AI27" s="60"/>
-      <c r="AJ27" s="60"/>
-      <c r="AK27" s="60"/>
-    </row>
-    <row r="28" spans="2:37" s="59" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="61">
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="58"/>
+      <c r="Y27" s="58"/>
+      <c r="Z27" s="58"/>
+      <c r="AA27" s="58"/>
+      <c r="AB27" s="58"/>
+      <c r="AC27" s="58"/>
+      <c r="AD27" s="58"/>
+      <c r="AE27" s="58"/>
+      <c r="AF27" s="58"/>
+      <c r="AG27" s="58"/>
+      <c r="AH27" s="58"/>
+      <c r="AI27" s="58"/>
+      <c r="AJ27" s="58"/>
+      <c r="AK27" s="58"/>
+    </row>
+    <row r="28" spans="2:37" s="57" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="59">
         <f t="shared" si="1"/>
         <v>0.59465772165882236</v>
       </c>
-      <c r="C28" s="67">
+      <c r="C28" s="65">
         <f t="shared" si="2"/>
         <v>0.42399095554274036</v>
       </c>
-      <c r="D28" s="61">
+      <c r="D28" s="59">
         <f t="shared" si="3"/>
         <v>-1.542776998597477E-2</v>
       </c>
-      <c r="I28" s="58" t="s">
+      <c r="I28" s="56" t="s">
         <v>358</v>
       </c>
-      <c r="J28" s="59">
+      <c r="J28" s="57">
         <v>0.71299999999999997</v>
       </c>
-      <c r="K28" s="62">
+      <c r="K28" s="60">
         <f>0.105*SQRT(L28)</f>
         <v>0.29698484809834996</v>
       </c>
-      <c r="L28" s="59">
+      <c r="L28" s="57">
         <v>8</v>
       </c>
-      <c r="M28" s="58" t="s">
+      <c r="M28" s="56" t="s">
         <v>300</v>
       </c>
-      <c r="N28" s="59">
+      <c r="N28" s="57">
         <v>0.70199999999999996</v>
       </c>
-      <c r="O28" s="62">
+      <c r="O28" s="60">
         <f>0.112*SQRT(P28)</f>
         <v>0.31678383797157333</v>
       </c>
-      <c r="P28" s="59">
+      <c r="P28" s="57">
         <v>8</v>
       </c>
-      <c r="Q28" s="59" t="s">
+      <c r="Q28" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="R28" s="59">
+      <c r="R28" s="57">
         <v>7</v>
       </c>
-      <c r="S28" s="59" t="s">
+      <c r="S28" s="57" t="s">
         <v>309</v>
       </c>
-      <c r="T28" s="58" t="s">
+      <c r="T28" s="56" t="s">
         <v>301</v>
       </c>
-      <c r="U28" s="60"/>
-      <c r="V28" s="60"/>
-      <c r="W28" s="60"/>
-      <c r="X28" s="60"/>
-      <c r="Y28" s="60"/>
-      <c r="Z28" s="60"/>
-      <c r="AA28" s="60"/>
-      <c r="AB28" s="60"/>
-      <c r="AC28" s="60"/>
-      <c r="AD28" s="60"/>
-      <c r="AE28" s="60"/>
-      <c r="AF28" s="60"/>
-      <c r="AG28" s="60"/>
-      <c r="AH28" s="60"/>
-      <c r="AI28" s="60"/>
-      <c r="AJ28" s="60"/>
-      <c r="AK28" s="60"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
+      <c r="W28" s="58"/>
+      <c r="X28" s="58"/>
+      <c r="Y28" s="58"/>
+      <c r="Z28" s="58"/>
+      <c r="AA28" s="58"/>
+      <c r="AB28" s="58"/>
+      <c r="AC28" s="58"/>
+      <c r="AD28" s="58"/>
+      <c r="AE28" s="58"/>
+      <c r="AF28" s="58"/>
+      <c r="AG28" s="58"/>
+      <c r="AH28" s="58"/>
+      <c r="AI28" s="58"/>
+      <c r="AJ28" s="58"/>
+      <c r="AK28" s="58"/>
     </row>
     <row r="29" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="61">
+      <c r="B29" s="59">
         <f t="shared" si="1"/>
         <v>0.62604580322464665</v>
       </c>
-      <c r="C29" s="67">
+      <c r="C29" s="65">
         <f t="shared" si="2"/>
         <v>5.5718076486993548E-2</v>
       </c>
-      <c r="D29" s="61">
+      <c r="D29" s="59">
         <f t="shared" si="3"/>
         <v>-0.3146067415730337</v>
       </c>
-      <c r="I29" s="58" t="s">
+      <c r="I29" s="56" t="s">
         <v>371</v>
       </c>
-      <c r="J29" s="59">
+      <c r="J29" s="57">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="K29" s="62">
+      <c r="K29" s="60">
         <f>0.01*SQRT(L29)</f>
         <v>3.7416573867739417E-2</v>
       </c>
-      <c r="L29" s="59">
+      <c r="L29" s="57">
         <v>14</v>
       </c>
-      <c r="M29" s="58" t="s">
+      <c r="M29" s="56" t="s">
         <v>372</v>
       </c>
-      <c r="N29" s="59">
+      <c r="N29" s="57">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="O29" s="62">
+      <c r="O29" s="60">
         <f>0.01*SQRT(P29)</f>
         <v>3.7416573867739417E-2</v>
       </c>
-      <c r="P29" s="59">
+      <c r="P29" s="57">
         <v>14</v>
       </c>
-      <c r="Q29" s="59" t="s">
+      <c r="Q29" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="R29" s="59">
+      <c r="R29" s="57">
         <v>1</v>
       </c>
-      <c r="S29" s="59" t="s">
+      <c r="S29" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T29" s="58" t="s">
+      <c r="T29" s="56" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="30" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="61">
+      <c r="B30" s="59">
         <f t="shared" si="1"/>
         <v>0.64173877726018158</v>
       </c>
-      <c r="C30" s="67">
+      <c r="C30" s="65">
         <f t="shared" si="2"/>
         <v>14.824165754710195</v>
       </c>
-      <c r="D30" s="61">
+      <c r="D30" s="59">
         <f t="shared" si="3"/>
         <v>-0.16017316017316027</v>
       </c>
-      <c r="I30" s="85" t="s">
+      <c r="I30" s="82" t="s">
         <v>390</v>
       </c>
-      <c r="J30" s="66">
+      <c r="J30" s="64">
         <v>23.1</v>
       </c>
-      <c r="K30" s="66">
+      <c r="K30" s="64">
         <v>11.3</v>
       </c>
-      <c r="L30" s="66">
+      <c r="L30" s="64">
         <v>7</v>
       </c>
-      <c r="M30" s="85" t="s">
+      <c r="M30" s="82" t="s">
         <v>391</v>
       </c>
-      <c r="N30" s="66">
+      <c r="N30" s="64">
         <v>19.399999999999999</v>
       </c>
-      <c r="O30" s="86">
+      <c r="O30" s="83">
         <v>7.15</v>
       </c>
-      <c r="P30" s="66">
+      <c r="P30" s="64">
         <v>8</v>
       </c>
-      <c r="Q30" s="66" t="s">
+      <c r="Q30" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="R30" s="66">
+      <c r="R30" s="64">
         <v>2</v>
       </c>
-      <c r="S30" s="66" t="s">
+      <c r="S30" s="64" t="s">
         <v>308</v>
       </c>
-      <c r="T30" s="65" t="s">
+      <c r="T30" s="63" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="31" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="61">
+      <c r="B31" s="59">
         <f t="shared" si="1"/>
         <v>0.72845716036649566</v>
       </c>
-      <c r="C31" s="63">
+      <c r="C31" s="61">
         <f t="shared" si="2"/>
         <v>47087.470846090277</v>
       </c>
-      <c r="D31" s="61">
+      <c r="D31" s="59">
         <f t="shared" si="3"/>
         <v>-0.16615099009900991</v>
       </c>
-      <c r="I31" s="58" t="s">
+      <c r="I31" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="J31" s="59">
+      <c r="J31" s="57">
         <v>64640</v>
       </c>
-      <c r="K31" s="59">
+      <c r="K31" s="57">
         <v>34390</v>
       </c>
-      <c r="L31" s="59">
+      <c r="L31" s="57">
         <v>9</v>
       </c>
-      <c r="M31" s="58" t="s">
+      <c r="M31" s="56" t="s">
         <v>266</v>
       </c>
-      <c r="N31" s="59">
+      <c r="N31" s="57">
         <v>53900</v>
       </c>
-      <c r="O31" s="59">
+      <c r="O31" s="57">
         <v>10830</v>
       </c>
-      <c r="P31" s="59">
+      <c r="P31" s="57">
         <v>10</v>
       </c>
-      <c r="Q31" s="59" t="s">
+      <c r="Q31" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R31" s="59">
+      <c r="R31" s="57">
         <v>21</v>
       </c>
-      <c r="S31" s="59" t="s">
+      <c r="S31" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T31" s="58" t="s">
+      <c r="T31" s="56" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="32" spans="2:37" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="61">
+      <c r="B32" s="59">
         <f t="shared" si="1"/>
         <v>0.87193649776221871</v>
       </c>
-      <c r="C32" s="63">
+      <c r="C32" s="61">
         <f t="shared" si="2"/>
         <v>265755.7812799511</v>
       </c>
-      <c r="D32" s="61">
+      <c r="D32" s="59">
         <f t="shared" si="3"/>
         <v>1.8032205992361904E-2</v>
       </c>
-      <c r="I32" s="58" t="s">
+      <c r="I32" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="J32" s="59">
+      <c r="J32" s="57">
         <v>304788</v>
       </c>
-      <c r="K32" s="59">
+      <c r="K32" s="57">
         <v>113425</v>
       </c>
-      <c r="L32" s="59">
+      <c r="L32" s="57">
         <v>4</v>
       </c>
-      <c r="M32" s="58" t="s">
+      <c r="M32" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="N32" s="59">
+      <c r="N32" s="57">
         <v>310284</v>
       </c>
-      <c r="O32" s="59">
+      <c r="O32" s="57">
         <v>160647</v>
       </c>
-      <c r="P32" s="59">
+      <c r="P32" s="57">
         <v>3</v>
       </c>
-      <c r="Q32" s="59" t="s">
+      <c r="Q32" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R32" s="59">
+      <c r="R32" s="57">
         <v>3</v>
       </c>
-      <c r="S32" s="59" t="s">
+      <c r="S32" s="57" t="s">
         <v>332</v>
       </c>
-      <c r="T32" s="71" t="s">
+      <c r="T32" s="69" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="33" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="61">
+      <c r="B33" s="59">
         <f t="shared" si="1"/>
         <v>0.90104148622149904</v>
       </c>
-      <c r="C33" s="63">
+      <c r="C33" s="61">
         <f t="shared" si="2"/>
         <v>202294.53605041257</v>
       </c>
-      <c r="D33" s="61">
+      <c r="D33" s="59">
         <f t="shared" si="3"/>
         <v>-0.22222385539474743</v>
       </c>
-      <c r="I33" s="58" t="s">
+      <c r="I33" s="56" t="s">
         <v>392</v>
       </c>
-      <c r="J33" s="59">
+      <c r="J33" s="57">
         <v>224511.9</v>
       </c>
-      <c r="K33" s="63">
+      <c r="K33" s="61">
         <f>(258134.5-J33)*SQRT(L33)</f>
         <v>82358.213825701692</v>
       </c>
-      <c r="L33" s="59">
+      <c r="L33" s="57">
         <v>6</v>
       </c>
-      <c r="M33" s="58" t="s">
+      <c r="M33" s="56" t="s">
         <v>393</v>
       </c>
-      <c r="N33" s="59">
+      <c r="N33" s="57">
         <v>174620</v>
       </c>
-      <c r="O33" s="63">
+      <c r="O33" s="61">
         <f>(215835-N33)*SQRT(P33)</f>
         <v>109044.6402855271</v>
       </c>
-      <c r="P33" s="59">
+      <c r="P33" s="57">
         <v>7</v>
       </c>
-      <c r="Q33" s="59" t="s">
+      <c r="Q33" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R33" s="59">
+      <c r="R33" s="57">
         <v>12</v>
       </c>
-      <c r="S33" s="59" t="s">
+      <c r="S33" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T33" s="58" t="s">
+      <c r="T33" s="56" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="34" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="61">
+      <c r="B34" s="59">
         <f t="shared" si="1"/>
         <v>0.93271875715240415</v>
       </c>
-      <c r="C34" s="63">
+      <c r="C34" s="61">
         <f t="shared" si="2"/>
         <v>60253.631712045302</v>
       </c>
-      <c r="D34" s="61">
+      <c r="D34" s="59">
         <f t="shared" si="3"/>
         <v>-0.16563467492260053</v>
       </c>
-      <c r="I34" s="58" t="s">
+      <c r="I34" s="56" t="s">
         <v>263</v>
       </c>
-      <c r="J34" s="59">
+      <c r="J34" s="57">
         <f>64.6*1000</f>
         <v>64599.999999999993</v>
       </c>
-      <c r="K34" s="59">
+      <c r="K34" s="57">
         <f>34.4*1000</f>
         <v>34400</v>
       </c>
-      <c r="L34" s="59">
+      <c r="L34" s="57">
         <v>9</v>
       </c>
-      <c r="M34" s="58" t="s">
+      <c r="M34" s="56" t="s">
         <v>264</v>
       </c>
-      <c r="N34" s="59">
+      <c r="N34" s="57">
         <f>53.9*1000</f>
         <v>53900</v>
       </c>
-      <c r="O34" s="59">
+      <c r="O34" s="57">
         <f>34.8*1000</f>
         <v>34800</v>
       </c>
-      <c r="P34" s="59">
+      <c r="P34" s="57">
         <v>9</v>
       </c>
-      <c r="Q34" s="59" t="s">
+      <c r="Q34" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R34" s="59">
+      <c r="R34" s="57">
         <v>21</v>
       </c>
-      <c r="S34" s="59" t="s">
+      <c r="S34" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T34" s="58" t="s">
+      <c r="T34" s="56" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="35" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="61">
+      <c r="B35" s="59">
         <f t="shared" si="1"/>
         <v>0.96814672232900045</v>
       </c>
-      <c r="C35" s="67">
+      <c r="C35" s="65">
         <f t="shared" si="2"/>
         <v>34.853282003844015</v>
       </c>
-      <c r="D35" s="61">
+      <c r="D35" s="59">
         <f t="shared" si="3"/>
         <v>0.1388888888888889</v>
       </c>
-      <c r="I35" s="58" t="s">
+      <c r="I35" s="56" t="s">
         <v>314</v>
       </c>
-      <c r="J35" s="59">
+      <c r="J35" s="57">
         <v>36</v>
       </c>
-      <c r="K35" s="63">
+      <c r="K35" s="61">
         <f>6*SQRT(L35)</f>
         <v>23.237900077244504</v>
       </c>
-      <c r="L35" s="59">
+      <c r="L35" s="57">
         <v>15</v>
       </c>
-      <c r="M35" s="58" t="s">
+      <c r="M35" s="56" t="s">
         <v>314</v>
       </c>
-      <c r="N35" s="59">
+      <c r="N35" s="57">
         <v>41</v>
       </c>
-      <c r="O35" s="63">
+      <c r="O35" s="61">
         <f>14*SQRT(P35)</f>
         <v>50.47771785649585</v>
       </c>
-      <c r="P35" s="59">
+      <c r="P35" s="57">
         <v>13</v>
       </c>
-      <c r="Q35" s="59" t="s">
+      <c r="Q35" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="R35" s="59">
+      <c r="R35" s="57">
         <v>1</v>
       </c>
-      <c r="S35" s="59" t="s">
+      <c r="S35" s="57" t="s">
         <v>312</v>
       </c>
-      <c r="T35" s="60" t="s">
+      <c r="T35" s="58" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="61">
+      <c r="B36" s="59">
         <f t="shared" si="1"/>
         <v>1.0072498831657288</v>
       </c>
-      <c r="C36" s="63">
+      <c r="C36" s="61">
         <f t="shared" si="2"/>
         <v>391.71947956315188</v>
       </c>
-      <c r="D36" s="61">
+      <c r="D36" s="59">
         <f t="shared" si="3"/>
         <v>-0.25739264592440209</v>
       </c>
-      <c r="I36" s="58" t="s">
+      <c r="I36" s="56" t="s">
         <v>375</v>
       </c>
-      <c r="J36" s="59">
+      <c r="J36" s="57">
         <v>388.9</v>
       </c>
-      <c r="K36" s="59">
+      <c r="K36" s="57">
         <v>347.3</v>
       </c>
-      <c r="L36" s="59">
+      <c r="L36" s="57">
         <v>6</v>
       </c>
-      <c r="M36" s="58" t="s">
+      <c r="M36" s="56" t="s">
         <v>376</v>
       </c>
-      <c r="N36" s="59">
+      <c r="N36" s="57">
         <v>288.8</v>
       </c>
-      <c r="O36" s="59">
+      <c r="O36" s="57">
         <v>110.5</v>
       </c>
-      <c r="P36" s="59">
+      <c r="P36" s="57">
         <v>6</v>
       </c>
-      <c r="Q36" s="59" t="s">
+      <c r="Q36" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="R36" s="59">
+      <c r="R36" s="57">
         <v>1</v>
       </c>
-      <c r="S36" s="59" t="s">
+      <c r="S36" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T36" s="58" t="s">
+      <c r="T36" s="56" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="37" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="61">
+      <c r="B37" s="59">
         <f t="shared" si="1"/>
         <v>1.0221261204613394</v>
       </c>
-      <c r="C37" s="63">
+      <c r="C37" s="61">
         <f t="shared" si="2"/>
         <v>38503.49095777866</v>
       </c>
-      <c r="D37" s="61">
+      <c r="D37" s="59">
         <f t="shared" si="3"/>
         <v>-0.2808601008760287</v>
       </c>
-      <c r="I37" s="58" t="s">
+      <c r="I37" s="56" t="s">
         <v>258</v>
       </c>
-      <c r="J37" s="87">
+      <c r="J37" s="84">
         <v>37670</v>
       </c>
-      <c r="K37" s="63">
+      <c r="K37" s="61">
         <v>29510</v>
       </c>
-      <c r="L37" s="59">
+      <c r="L37" s="57">
         <v>9</v>
       </c>
-      <c r="M37" s="58" t="s">
+      <c r="M37" s="56" t="s">
         <v>259</v>
       </c>
-      <c r="N37" s="59">
+      <c r="N37" s="57">
         <v>27090</v>
       </c>
-      <c r="O37" s="63">
+      <c r="O37" s="61">
         <v>29150</v>
       </c>
-      <c r="P37" s="59">
+      <c r="P37" s="57">
         <v>8</v>
       </c>
-      <c r="Q37" s="59" t="s">
+      <c r="Q37" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R37" s="59">
+      <c r="R37" s="57">
         <v>1</v>
       </c>
-      <c r="S37" s="59" t="s">
+      <c r="S37" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T37" s="58" t="s">
+      <c r="T37" s="56" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="38" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="61">
+      <c r="B38" s="59">
         <f t="shared" si="1"/>
         <v>1.0559803904811791</v>
       </c>
-      <c r="C38" s="63">
+      <c r="C38" s="61">
         <f t="shared" si="2"/>
         <v>68258.572440703414</v>
       </c>
-      <c r="D38" s="61">
+      <c r="D38" s="59">
         <f t="shared" si="3"/>
         <v>-0.45730198019801982</v>
       </c>
-      <c r="I38" s="58" t="s">
+      <c r="I38" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="J38" s="59">
+      <c r="J38" s="57">
         <v>64640</v>
       </c>
-      <c r="K38" s="59">
+      <c r="K38" s="57">
         <v>34390</v>
       </c>
-      <c r="L38" s="59">
+      <c r="L38" s="57">
         <v>9</v>
       </c>
-      <c r="M38" s="58" t="s">
+      <c r="M38" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="N38" s="59">
+      <c r="N38" s="57">
         <v>35080</v>
       </c>
-      <c r="O38" s="59">
+      <c r="O38" s="57">
         <v>18420</v>
       </c>
-      <c r="P38" s="59">
+      <c r="P38" s="57">
         <v>11</v>
       </c>
-      <c r="Q38" s="59" t="s">
+      <c r="Q38" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R38" s="59">
+      <c r="R38" s="57">
         <v>21</v>
       </c>
-      <c r="S38" s="59" t="s">
+      <c r="S38" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T38" s="58" t="s">
+      <c r="T38" s="56" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="39" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="61">
+      <c r="B39" s="59">
         <v>1.0644902360012614</v>
       </c>
-      <c r="C39" s="59">
+      <c r="C39" s="57">
         <v>26665.480411831599</v>
       </c>
-      <c r="D39" s="59">
+      <c r="D39" s="57">
         <v>0.36167664670658684</v>
       </c>
-      <c r="I39" s="58" t="s">
+      <c r="I39" s="56" t="s">
         <v>394</v>
       </c>
-      <c r="J39" s="59">
+      <c r="J39" s="57">
         <v>25050</v>
       </c>
-      <c r="K39" s="59">
+      <c r="K39" s="57">
         <v>22192.377069615592</v>
       </c>
-      <c r="L39" s="59">
+      <c r="L39" s="57">
         <v>24</v>
       </c>
-      <c r="M39" s="58" t="s">
+      <c r="M39" s="56" t="s">
         <v>395</v>
       </c>
-      <c r="N39" s="59">
+      <c r="N39" s="57">
         <v>34110</v>
       </c>
-      <c r="O39" s="59">
+      <c r="O39" s="57">
         <v>22454.620905283617</v>
       </c>
-      <c r="P39" s="59">
+      <c r="P39" s="57">
         <v>21</v>
       </c>
-      <c r="Q39" s="59" t="s">
+      <c r="Q39" s="57" t="s">
         <v>353</v>
       </c>
-      <c r="R39" s="59">
+      <c r="R39" s="57">
         <v>6</v>
       </c>
-      <c r="S39" s="59" t="s">
+      <c r="S39" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T39" s="58" t="s">
+      <c r="T39" s="56" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="40" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="61">
+      <c r="B40" s="59">
         <f>C40/J40</f>
         <v>1.1601979569426732</v>
       </c>
-      <c r="C40" s="68">
+      <c r="C40" s="66">
         <f>ABS(N40-J40) + ABS(_xlfn.NORM.S.INV(1-(0.05/R40)/2))*SQRT(K40^2/L40+O40^2/P40)</f>
         <v>24.654206585031805</v>
       </c>
-      <c r="D40" s="61">
+      <c r="D40" s="59">
         <f>-(J40-N40)/J40</f>
         <v>-0.34211764705882353</v>
       </c>
-      <c r="I40" s="58" t="s">
+      <c r="I40" s="56" t="s">
         <v>371</v>
       </c>
-      <c r="J40" s="59">
+      <c r="J40" s="57">
         <v>21.25</v>
       </c>
-      <c r="K40" s="68">
+      <c r="K40" s="66">
         <f>(28.63-J40)*SQRT(L40)</f>
         <v>18.07723430173985</v>
       </c>
-      <c r="L40" s="59">
+      <c r="L40" s="57">
         <v>6</v>
       </c>
-      <c r="M40" s="58" t="s">
+      <c r="M40" s="56" t="s">
         <v>396</v>
       </c>
-      <c r="N40" s="59">
+      <c r="N40" s="57">
         <v>13.98</v>
       </c>
-      <c r="O40" s="68">
+      <c r="O40" s="66">
         <f>(18.9-N40)*SQRT(P40)</f>
         <v>12.05148953449323</v>
       </c>
-      <c r="P40" s="59">
+      <c r="P40" s="57">
         <v>6</v>
       </c>
-      <c r="Q40" s="59" t="s">
+      <c r="Q40" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="R40" s="59">
+      <c r="R40" s="57">
         <v>1</v>
       </c>
-      <c r="S40" s="59" t="s">
+      <c r="S40" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T40" s="58" t="s">
+      <c r="T40" s="56" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="61">
+      <c r="B41" s="59">
         <f>C41/J41</f>
         <v>1.3730702180767695</v>
       </c>
-      <c r="C41" s="67">
+      <c r="C41" s="65">
         <f>ABS(N41-J41) + ABS(_xlfn.NORM.S.INV(1-(0.05/R41)/2))*SQRT(K41^2/L41+O41^2/P41)</f>
         <v>0.23754114772728113</v>
       </c>
-      <c r="D41" s="61">
+      <c r="D41" s="59">
         <f>-(J41-N41)/J41</f>
         <v>-0.51445086705202303</v>
       </c>
-      <c r="I41" s="58" t="s">
+      <c r="I41" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="J41" s="59">
+      <c r="J41" s="57">
         <v>0.17299999999999999</v>
       </c>
-      <c r="K41" s="62">
+      <c r="K41" s="60">
         <f>(0.226-J41)*SQRT(L41)</f>
         <v>0.14990663761154813</v>
       </c>
-      <c r="L41" s="59">
+      <c r="L41" s="57">
         <v>8</v>
       </c>
-      <c r="M41" s="58" t="s">
+      <c r="M41" s="56" t="s">
         <v>302</v>
       </c>
-      <c r="N41" s="59">
+      <c r="N41" s="57">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="O41" s="67">
+      <c r="O41" s="65">
         <f>(0.103-N41)*SQRT(P41)</f>
         <v>5.3740115370177588E-2</v>
       </c>
-      <c r="P41" s="59">
+      <c r="P41" s="57">
         <v>8</v>
       </c>
-      <c r="Q41" s="59" t="s">
+      <c r="Q41" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="R41" s="59">
+      <c r="R41" s="57">
         <v>6</v>
       </c>
-      <c r="S41" s="59" t="s">
+      <c r="S41" s="57" t="s">
         <v>309</v>
       </c>
-      <c r="T41" s="58" t="s">
+      <c r="T41" s="56" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="42" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="61">
+      <c r="B42" s="59">
         <f>C42/J42</f>
         <v>1.407364705439331</v>
       </c>
-      <c r="C42" s="68">
+      <c r="C42" s="66">
         <f>ABS(N42-J42) + ABS(_xlfn.NORM.S.INV(1-(0.05/R42)/2))*SQRT(K42^2/L42+O42^2/P42)</f>
         <v>83.175254091464467</v>
       </c>
-      <c r="D42" s="61">
+      <c r="D42" s="59">
         <f>-(J42-N42)/J42</f>
         <v>-8.1218274111675204E-2</v>
       </c>
-      <c r="I42" s="58" t="s">
+      <c r="I42" s="56" t="s">
         <v>256</v>
       </c>
-      <c r="J42" s="59">
+      <c r="J42" s="57">
         <v>59.1</v>
       </c>
-      <c r="K42" s="63">
+      <c r="K42" s="61">
         <v>63.8</v>
       </c>
-      <c r="L42" s="59">
+      <c r="L42" s="57">
         <v>6</v>
       </c>
-      <c r="M42" s="58" t="s">
+      <c r="M42" s="56" t="s">
         <v>257</v>
       </c>
-      <c r="N42" s="59">
+      <c r="N42" s="57">
         <v>54.3</v>
       </c>
-      <c r="O42" s="59">
+      <c r="O42" s="57">
         <v>56.1</v>
       </c>
-      <c r="P42" s="59">
+      <c r="P42" s="57">
         <v>8</v>
       </c>
-      <c r="Q42" s="59" t="s">
+      <c r="Q42" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="R42" s="59">
+      <c r="R42" s="57">
         <v>3</v>
       </c>
-      <c r="S42" s="59" t="s">
+      <c r="S42" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T42" s="58" t="s">
+      <c r="T42" s="56" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="43" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="61">
+      <c r="B43" s="59">
         <f>C43/J43</f>
         <v>1.8080937690781533</v>
       </c>
-      <c r="C43" s="63">
+      <c r="C43" s="61">
         <f>ABS(N43-J43) + ABS(_xlfn.NORM.S.INV(1-(0.05/R43)/2))*SQRT(K43^2/L43+O43^2/P43)</f>
         <v>18001.381564942094</v>
       </c>
-      <c r="D43" s="61">
+      <c r="D43" s="59">
         <f>-(J43-N43)/J43</f>
         <v>0.72719967858577739</v>
       </c>
-      <c r="I43" s="58" t="s">
+      <c r="I43" s="56" t="s">
         <v>397</v>
       </c>
-      <c r="J43" s="59">
+      <c r="J43" s="57">
         <v>9956</v>
       </c>
-      <c r="K43" s="63">
+      <c r="K43" s="61">
         <f>(12545-J43)*SQRT(L43)</f>
         <v>11578.359987493912</v>
       </c>
-      <c r="L43" s="59">
+      <c r="L43" s="57">
         <v>20</v>
       </c>
-      <c r="M43" s="58" t="s">
+      <c r="M43" s="56" t="s">
         <v>398</v>
       </c>
-      <c r="N43" s="59">
+      <c r="N43" s="57">
         <v>17196</v>
       </c>
-      <c r="O43" s="63">
+      <c r="O43" s="61">
         <f>(20348-N43)*SQRT(P43)</f>
         <v>13372.803445799986</v>
       </c>
-      <c r="P43" s="59">
+      <c r="P43" s="57">
         <v>18</v>
       </c>
-      <c r="Q43" s="59" t="s">
+      <c r="Q43" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="R43" s="59">
+      <c r="R43" s="57">
         <v>6</v>
       </c>
-      <c r="S43" s="59" t="s">
+      <c r="S43" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T43" s="58" t="s">
+      <c r="T43" s="56" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="44" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="61">
+      <c r="B44" s="59">
         <f>C44/J44</f>
         <v>0.91051281258890382</v>
       </c>
-      <c r="C44" s="68">
+      <c r="C44" s="66">
         <f>ABS(N44-J44) + ABS(_xlfn.NORM.S.INV(1-(0.05/R44)/2))*SQRT(K44^2/L44+O44^2/P44)</f>
         <v>10.052061450981498</v>
       </c>
-      <c r="D44" s="61">
+      <c r="D44" s="59">
         <f>-(J44-N44)/J44</f>
         <v>-0.30706521739130427</v>
       </c>
-      <c r="I44" s="58" t="s">
+      <c r="I44" s="56" t="s">
         <v>371</v>
       </c>
-      <c r="J44" s="59">
+      <c r="J44" s="57">
         <v>11.04</v>
       </c>
-      <c r="K44" s="59">
+      <c r="K44" s="57">
         <f>(15-J44)</f>
         <v>3.9600000000000009</v>
       </c>
-      <c r="L44" s="59">
+      <c r="L44" s="57">
         <v>6</v>
       </c>
-      <c r="M44" s="58" t="s">
+      <c r="M44" s="56" t="s">
         <v>396</v>
       </c>
-      <c r="N44" s="59">
+      <c r="N44" s="57">
         <v>7.65</v>
       </c>
-      <c r="O44" s="68">
+      <c r="O44" s="66">
         <f>(10.64-N44)*SQRT(P44)</f>
         <v>7.3239743309217022</v>
       </c>
-      <c r="P44" s="59">
+      <c r="P44" s="57">
         <v>6</v>
       </c>
-      <c r="Q44" s="59" t="s">
+      <c r="Q44" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="R44" s="59">
+      <c r="R44" s="57">
         <v>1</v>
       </c>
-      <c r="S44" s="59" t="s">
+      <c r="S44" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="T44" s="58" t="s">
+      <c r="T44" s="56" t="s">
         <v>295</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I23:P26 R23:R26 I27:R27 I28:P28 J29:P29 J31:L31 N31:P31 I32:I33 I33:P33 J35:L35 N35:R35 I36:P36 J37:L38 R28 K32:R32 I22:R22 R31 R36 N37:R38 R33:R34 V39:XFD39 L40:P40 I41:P41 R40 I42:R42 T36:T38 T21:T22 T28:T34 U41:XFD1048576 U21:XFD38 T40:XFD40 T19:XFD20 J43:L43 N43:S43 R44 L44:P44 C12 V15:XFD15 V8:V11 Y3:Y6 Y8:Y11 V5:X6 W7 I40:J40 I19:R20 C1:D1 I1:XFD1 I45:T1048576 I16:XFD18 I39:T39 T5 E3 I6:P7 R6:R7 I11:T11 E5:E7 Q2:T2 V2:XFD2 W4:X4 I14:XFD14 I12:AC13 AI8:XFD13 B45:D1048576 B16:D19 B39:D40 B3:C3 H3:H8 E8:G8 H11:H12 E11:E12 E11:G11 B13:H14 E16:H1048576 E9:H10 AA8:AC11 AA3:XFD7 W8:X10 B5:C11">
+  <conditionalFormatting sqref="I23:P26 R23:R26 I27:R27 I28:P28 J29:P29 J31:L31 N31:P31 I32:I33 I33:P33 J35:L35 N35:R35 I36:P36 J37:L38 R28 K32:R32 I22:R22 R31 R36 N37:R38 R33:R34 V39:XFD39 L40:P40 I41:P41 R40 I42:R42 T36:T38 T21:T22 T28:T34 U41:XFD1048576 U21:XFD38 T40:XFD40 T19:XFD20 J43:L43 N43:S43 R44 L44:P44 C12 V8:V11 Y3:Y6 Y8:Y11 V5:X6 W7 I40:J40 I19:R20 C1:D1 I1:XFD1 I45:T1048576 I16:XFD18 I39:T39 T5 E3 I6:P7 R6:R7 I11:T11 E5:E7 Q2:T2 V2:XFD2 W4:X4 V14:XFD15 I12:AC13 AI8:XFD13 B45:D1048576 B16:D19 B39:D40 B3:C3 H11:H12 E11:E12 E11:G11 E16:H1048576 AA8:AC11 AA3:XFD7 W8:X10 H3:H7 F7 E10:H10 E8:H8 B10:C11 B5:C8 B13:H13 B9:H9">
     <cfRule type="expression" dxfId="566" priority="521">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -16889,7 +16956,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
+  <conditionalFormatting sqref="D8">
     <cfRule type="expression" dxfId="299" priority="168">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -16958,7 +17025,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="D9">
     <cfRule type="expression" dxfId="282" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -16966,7 +17033,7 @@
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:H1 F5:G7 F7:F8">
+  <conditionalFormatting sqref="E1:H1 F5:G7">
     <cfRule type="expression" dxfId="280" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17045,15 +17112,15 @@
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="expression" dxfId="261" priority="64">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="260" priority="65">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="261" priority="64">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="260" priority="65">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
     <cfRule type="expression" dxfId="259" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17061,7 +17128,7 @@
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+  <conditionalFormatting sqref="C9">
     <cfRule type="expression" dxfId="257" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17069,7 +17136,7 @@
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
+  <conditionalFormatting sqref="B9">
     <cfRule type="expression" dxfId="255" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17210,7 +17277,7 @@
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U8">
+  <conditionalFormatting sqref="U9">
     <cfRule type="expression" dxfId="220" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17226,7 +17293,7 @@
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U9">
+  <conditionalFormatting sqref="U8">
     <cfRule type="expression" dxfId="216" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17338,44 +17405,44 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="111" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+    <row r="2" spans="1:15" s="108" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="105" t="s">
         <v>361</v>
       </c>
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="106" t="s">
         <v>422</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="105" t="s">
         <v>427</v>
       </c>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="105" t="s">
         <v>428</v>
       </c>
-      <c r="E2" s="108" t="s">
+      <c r="E2" s="105" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="109" t="s">
+      <c r="F2" s="106" t="s">
         <v>429</v>
       </c>
-      <c r="G2" s="108" t="s">
+      <c r="G2" s="105" t="s">
         <v>424</v>
       </c>
-      <c r="H2" s="108" t="s">
+      <c r="H2" s="105" t="s">
         <v>425</v>
       </c>
-      <c r="I2" s="108" t="s">
+      <c r="I2" s="105" t="s">
         <v>426</v>
       </c>
-      <c r="J2" s="108" t="s">
+      <c r="J2" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="108" t="s">
+      <c r="K2" s="105" t="s">
         <v>362</v>
       </c>
-      <c r="L2" s="108" t="s">
+      <c r="L2" s="105" t="s">
         <v>303</v>
       </c>
-      <c r="M2" s="109" t="s">
+      <c r="M2" s="106" t="s">
         <v>172</v>
       </c>
     </row>
@@ -19482,31 +19549,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="H2" s="122" t="s">
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="H2" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122" t="s">
+      <c r="I2" s="119"/>
+      <c r="J2" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="122"/>
+      <c r="K2" s="119"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="122" t="s">
+      <c r="N2" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="122"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="122"/>
-      <c r="R2" s="122"/>
-      <c r="S2" s="122"/>
-      <c r="T2" s="122"/>
+      <c r="O2" s="119"/>
+      <c r="P2" s="119"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="119"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
     </row>
     <row r="3" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">

</xml_diff>